<commit_message>
modify hanwudi field in chinaHistory xlsx
</commit_message>
<xml_diff>
--- a/中国史卷/中国史卷.xlsx
+++ b/中国史卷/中国史卷.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="570" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="560" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="电子表格1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4478" uniqueCount="4478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4547" uniqueCount="4547">
   <si>
     <t>B.C</t>
   </si>
@@ -13524,6 +13524,243 @@
 汉武帝
 世宗
 54</t>
+  </si>
+  <si>
+    <t>长平之战</t>
+  </si>
+  <si>
+    <t>秦赵长平之战</t>
+  </si>
+  <si>
+    <t>商鞅变法</t>
+  </si>
+  <si>
+    <t>巨鹿之战</t>
+  </si>
+  <si>
+    <t>董仲舒“”</t>
+  </si>
+  <si>
+    <t>董仲舒“天人三策”</t>
+  </si>
+  <si>
+    <t>董仲舒“天人三策”
+罢黜百家，独尊儒术</t>
+  </si>
+  <si>
+    <t>淮南王刘安自杀</t>
+  </si>
+  <si>
+    <t>诏纳敢谏之士</t>
+  </si>
+  <si>
+    <t>诏纳敢谏之士
+董仲舒</t>
+  </si>
+  <si>
+    <t>严助</t>
+  </si>
+  <si>
+    <t>诏纳敢谏之士
+董仲舒
+严助</t>
+  </si>
+  <si>
+    <t>向商贾征车船税</t>
+  </si>
+  <si>
+    <t>以巫蛊罪废陈阿娇皇后位</t>
+  </si>
+  <si>
+    <t>灌夫族诛
+窦婴弃世</t>
+  </si>
+  <si>
+    <t>推恩令</t>
+  </si>
+  <si>
+    <t>推恩令
+齐王“禽兽行”自杀</t>
+  </si>
+  <si>
+    <t>推恩令
+齐王“禽兽行”自杀
+齐相主父偃族诛</t>
+  </si>
+  <si>
+    <t>推恩令
+齐王“禽兽行”自杀
+齐相主父偃族诛
+燕王“禽兽行”自杀</t>
+  </si>
+  <si>
+    <t>颁令可买爵赎罪</t>
+  </si>
+  <si>
+    <t>淮南王刘安自杀
+衡王刘赐自杀</t>
+  </si>
+  <si>
+    <t>汉军征匈奴</t>
+  </si>
+  <si>
+    <t>汉军征匈奴
+董仲舒辞官</t>
+  </si>
+  <si>
+    <t>盐铁专营
+李广自杀</t>
+  </si>
+  <si>
+    <t>创腹诽罪</t>
+  </si>
+  <si>
+    <t>张汤自杀</t>
+  </si>
+  <si>
+    <t>下告缗令</t>
+  </si>
+  <si>
+    <t>董仲舒死</t>
+  </si>
+  <si>
+    <t>发七科谪</t>
+  </si>
+  <si>
+    <t>司马迁受宫刑</t>
+  </si>
+  <si>
+    <t>酒水官营</t>
+  </si>
+  <si>
+    <t>江充灭族</t>
+  </si>
+  <si>
+    <t>公孙贺族诛</t>
+  </si>
+  <si>
+    <t>公孙贺族诛
+卫伉被杀</t>
+  </si>
+  <si>
+    <t>下《》</t>
+  </si>
+  <si>
+    <t>下《轮台罪己诏》</t>
+  </si>
+  <si>
+    <t>赵敬肃王彭祖薨</t>
+  </si>
+  <si>
+    <t>赵敬肃王彭祖薨，武始侯刘昌继位</t>
+  </si>
+  <si>
+    <t>发七科谪
+发李广利出击匈奴</t>
+  </si>
+  <si>
+    <t>发七科谪
+发李广利出击匈奴
+李陵族诛</t>
+  </si>
+  <si>
+    <t>立刘髆为昌邑王</t>
+  </si>
+  <si>
+    <t>赦天下</t>
+  </si>
+  <si>
+    <t>匈奴犯雁门关</t>
+  </si>
+  <si>
+    <t>且鞮侯单于身死</t>
+  </si>
+  <si>
+    <t>且鞮侯单于身死，狐鹿孤单于继位</t>
+  </si>
+  <si>
+    <t>且鞮侯单于身死，狐鹿姑单于继位</t>
+  </si>
+  <si>
+    <t>穿渠引泾水</t>
+  </si>
+  <si>
+    <t>武帝东巡</t>
+  </si>
+  <si>
+    <t>生刘弗陵</t>
+  </si>
+  <si>
+    <t>武帝幸泰山</t>
+  </si>
+  <si>
+    <t>日食</t>
+  </si>
+  <si>
+    <t>卫伉被杀</t>
+  </si>
+  <si>
+    <t>匈奴入上谷、五原</t>
+  </si>
+  <si>
+    <t>江充灭族
+匈奴犯五原</t>
+  </si>
+  <si>
+    <t>李广利出征</t>
+  </si>
+  <si>
+    <t>赦天下
+李广利被李陵所俘</t>
+  </si>
+  <si>
+    <t>赦天下</t>
+  </si>
+  <si>
+    <t>刘屈氂腰斩
+李广利家人收监</t>
+  </si>
+  <si>
+    <t>刘屈氂腰斩
+李广利家人收监，李广利降，家人族诛</t>
+  </si>
+  <si>
+    <t>公孙勇起兵，旋被杀</t>
+  </si>
+  <si>
+    <t>武帝东巡
+下《轮台罪己诏》</t>
+  </si>
+  <si>
+    <t>日食
+匈奴阏氏杀李广利</t>
+  </si>
+  <si>
+    <t>地震</t>
+  </si>
+  <si>
+    <t>地震
+武帝赐死刘弗陵之母赵婕侸</t>
+  </si>
+  <si>
+    <t>地震
+武帝赐死刘弗陵之母钩弋夫人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+立刘弗陵为太子
+命霍光辅政</t>
+  </si>
+  <si>
+    <t>赦天下
+济北王刘宽“禽兽行”自杀</t>
+  </si>
+  <si>
+    <t>匈奴入朔方</t>
+  </si>
+  <si>
+    <t>灌夫族诛
+窦婴弃市</t>
   </si>
 </sst>
 </file>
@@ -13533,7 +13770,7 @@
   <numFmts count="1">
     <numFmt numFmtId="64" formatCode="&quot;¥&quot;#,##0;\\\-&quot;¥&quot;#,##0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11.0"/>
       <name val="宋体"/>
@@ -13647,12 +13884,7 @@
     <font>
       <sz val="11.0"/>
       <name val="宋体"/>
-      <color rgb="FFFF0000"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <name val="宋体"/>
-      <color/>
+      <color rgb="FF000000"/>
     </font>
   </fonts>
   <fills count="34">
@@ -13853,10 +14085,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFC4700"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -14101,6 +14334,46 @@
         <color rgb="FF000000"/>
       </diagonal>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -14251,7 +14524,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -14459,22 +14732,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14487,6 +14760,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -14810,10 +15125,10 @@
   <dimension ref="A1:Y4115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C1923" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D1935" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H1949" sqref="H1949"/>
+      <selection pane="bottomRight" activeCell="H1950" sqref="H1950"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.500000"/>
@@ -14823,15 +15138,15 @@
     <col min="3" max="3" style="22" width="9.81138717" customWidth="1" outlineLevel="0"/>
     <col min="4" max="4" style="58" width="11.69723045" customWidth="1" outlineLevel="0"/>
     <col min="5" max="5" style="22" width="9.05704891" customWidth="1" outlineLevel="0"/>
-    <col min="6" max="6" style="22" width="22.25795375" customWidth="1" outlineLevel="0"/>
+    <col min="6" max="6" style="79" width="22.25795375" customWidth="1" outlineLevel="0"/>
     <col min="7" max="7" style="22" width="15.21747218" customWidth="1" outlineLevel="0"/>
     <col min="8" max="8" style="22" width="21.12644779" customWidth="1" outlineLevel="0"/>
     <col min="9" max="9" style="22" width="13.33162795" customWidth="1" outlineLevel="0"/>
     <col min="10" max="10" style="22" width="19.36632739" customWidth="1" outlineLevel="0"/>
-    <col min="11" max="11" style="22" width="13.08018218" customWidth="1" outlineLevel="0"/>
+    <col min="11" max="11" style="22" width="17.22903835" customWidth="1" outlineLevel="0"/>
     <col min="12" max="12" style="22" width="13.20590507" customWidth="1" outlineLevel="0"/>
     <col min="13" max="13" style="22" width="19.36632739" customWidth="1" outlineLevel="0"/>
-    <col min="14" max="14" style="22" width="15.34319507" customWidth="1" outlineLevel="0"/>
+    <col min="14" max="14" style="22" width="17.35476123" customWidth="1" outlineLevel="0"/>
     <col min="15" max="15" style="22" width="17.10331546" customWidth="1" outlineLevel="0"/>
     <col min="16" max="16" style="22" width="19.36632739" customWidth="1" outlineLevel="0"/>
     <col min="17" max="17" style="22" width="16.97759258" customWidth="1" outlineLevel="0"/>
@@ -14897,7 +15212,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="80" t="s">
         <v>4316</v>
       </c>
       <c r="G2" s="55" t="s">
@@ -25209,97 +25524,100 @@
       </c>
       <c r="B1712" s="3"/>
     </row>
-    <row r="1713" spans="1:2">
+    <row r="1713" spans="1:6">
       <c r="A1713" s="58" t="s">
         <v>3970</v>
       </c>
       <c r="B1713" s="3"/>
     </row>
-    <row r="1714" spans="1:2">
+    <row r="1714" spans="1:6">
       <c r="A1714" s="58" t="s">
         <v>3971</v>
       </c>
       <c r="B1714" s="3"/>
     </row>
-    <row r="1715" spans="1:2">
+    <row r="1715" spans="1:6">
       <c r="A1715" s="58" t="s">
         <v>3972</v>
       </c>
       <c r="B1715" s="3"/>
     </row>
-    <row r="1716" spans="1:2">
+    <row r="1716" spans="1:6">
       <c r="A1716" s="58" t="s">
         <v>3973</v>
       </c>
       <c r="B1716" s="3"/>
     </row>
-    <row r="1717" spans="1:2">
+    <row r="1717" spans="1:6">
       <c r="A1717" s="58" t="s">
         <v>3974</v>
       </c>
       <c r="B1717" s="3"/>
-    </row>
-    <row r="1718" spans="1:2">
+      <c r="F1717" s="79" t="s">
+        <v>4480</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:6">
       <c r="A1718" s="58" t="s">
         <v>3975</v>
       </c>
       <c r="B1718" s="3"/>
     </row>
-    <row r="1719" spans="1:2">
+    <row r="1719" spans="1:6">
       <c r="A1719" s="58" t="s">
         <v>3976</v>
       </c>
       <c r="B1719" s="3"/>
     </row>
-    <row r="1720" spans="1:2">
+    <row r="1720" spans="1:6">
       <c r="A1720" s="58" t="s">
         <v>3977</v>
       </c>
       <c r="B1720" s="3"/>
     </row>
-    <row r="1721" spans="1:2">
+    <row r="1721" spans="1:6">
       <c r="A1721" s="58" t="s">
         <v>3978</v>
       </c>
       <c r="B1721" s="3"/>
     </row>
-    <row r="1722" spans="1:2">
+    <row r="1722" spans="1:6">
       <c r="A1722" s="58" t="s">
         <v>3979</v>
       </c>
       <c r="B1722" s="3"/>
     </row>
-    <row r="1723" spans="1:2">
+    <row r="1723" spans="1:6">
       <c r="A1723" s="58" t="s">
         <v>3980</v>
       </c>
       <c r="B1723" s="3"/>
     </row>
-    <row r="1724" spans="1:2">
+    <row r="1724" spans="1:6">
       <c r="A1724" s="58" t="s">
         <v>3981</v>
       </c>
       <c r="B1724" s="3"/>
     </row>
-    <row r="1725" spans="1:2">
+    <row r="1725" spans="1:6">
       <c r="A1725" s="58" t="s">
         <v>3982</v>
       </c>
       <c r="B1725" s="3"/>
     </row>
-    <row r="1726" spans="1:2">
+    <row r="1726" spans="1:6">
       <c r="A1726" s="58" t="s">
         <v>3983</v>
       </c>
       <c r="B1726" s="3"/>
     </row>
-    <row r="1727" spans="1:2">
+    <row r="1727" spans="1:6">
       <c r="A1727" s="58" t="s">
         <v>3984</v>
       </c>
       <c r="B1727" s="3"/>
     </row>
-    <row r="1728" spans="1:2">
+    <row r="1728" spans="1:6">
       <c r="A1728" s="58" t="s">
         <v>3985</v>
       </c>
@@ -25814,6 +26132,9 @@
         <v>4070</v>
       </c>
       <c r="B1813" s="3"/>
+      <c r="F1813" s="79" t="s">
+        <v>4479</v>
+      </c>
     </row>
     <row r="1814" spans="1:17">
       <c r="A1814" s="58" t="s">
@@ -26102,7 +26423,7 @@
       <c r="C1855" s="62"/>
       <c r="D1855" s="3"/>
       <c r="E1855" s="3"/>
-      <c r="F1855" s="53"/>
+      <c r="F1855" s="81"/>
       <c r="G1855" s="53"/>
       <c r="H1855" s="53"/>
       <c r="I1855" s="53"/>
@@ -26125,7 +26446,7 @@
       <c r="C1856" s="62"/>
       <c r="D1856" s="3"/>
       <c r="E1856" s="3"/>
-      <c r="F1856" s="53" t="s">
+      <c r="F1856" s="81" t="s">
         <v>4302</v>
       </c>
       <c r="G1856" s="53"/>
@@ -26150,7 +26471,7 @@
       <c r="C1857" s="62"/>
       <c r="D1857" s="3"/>
       <c r="E1857" s="3"/>
-      <c r="F1857" s="53" t="s">
+      <c r="F1857" s="81" t="s">
         <v>4303</v>
       </c>
       <c r="G1857" s="53"/>
@@ -26175,7 +26496,7 @@
       <c r="C1858" s="62"/>
       <c r="D1858" s="3"/>
       <c r="E1858" s="3"/>
-      <c r="F1858" s="53"/>
+      <c r="F1858" s="81"/>
       <c r="G1858" s="53"/>
       <c r="H1858" s="53"/>
       <c r="I1858" s="53"/>
@@ -26198,7 +26519,7 @@
       <c r="C1859" s="62"/>
       <c r="D1859" s="3"/>
       <c r="E1859" s="3"/>
-      <c r="F1859" s="53" t="s">
+      <c r="F1859" s="81" t="s">
         <v>4300</v>
       </c>
       <c r="G1859" s="53"/>
@@ -26223,7 +26544,7 @@
       <c r="C1860" s="62"/>
       <c r="D1860" s="3"/>
       <c r="E1860" s="3"/>
-      <c r="F1860" s="53" t="s">
+      <c r="F1860" s="81" t="s">
         <v>4301</v>
       </c>
       <c r="G1860" s="53"/>
@@ -26248,7 +26569,7 @@
       <c r="C1861" s="62"/>
       <c r="D1861" s="3"/>
       <c r="E1861" s="3"/>
-      <c r="F1861" s="53"/>
+      <c r="F1861" s="81"/>
       <c r="G1861" s="53"/>
       <c r="H1861" s="53"/>
       <c r="I1861" s="53"/>
@@ -26271,7 +26592,7 @@
       <c r="C1862" s="62"/>
       <c r="D1862" s="3"/>
       <c r="E1862" s="3"/>
-      <c r="F1862" s="53" t="s">
+      <c r="F1862" s="81" t="s">
         <v>4448</v>
       </c>
       <c r="G1862" s="53"/>
@@ -26296,7 +26617,7 @@
       <c r="C1863" s="62"/>
       <c r="D1863" s="3"/>
       <c r="E1863" s="3"/>
-      <c r="F1863" s="53" t="s">
+      <c r="F1863" s="81" t="s">
         <v>4297</v>
       </c>
       <c r="G1863" s="53"/>
@@ -26321,7 +26642,7 @@
       <c r="C1864" s="62"/>
       <c r="D1864" s="3"/>
       <c r="E1864" s="3"/>
-      <c r="F1864" s="53"/>
+      <c r="F1864" s="81"/>
       <c r="G1864" s="53"/>
       <c r="H1864" s="53"/>
       <c r="I1864" s="53"/>
@@ -26344,7 +26665,7 @@
       <c r="C1865" s="62"/>
       <c r="D1865" s="3"/>
       <c r="E1865" s="3"/>
-      <c r="F1865" s="53"/>
+      <c r="F1865" s="81"/>
       <c r="G1865" s="53"/>
       <c r="H1865" s="53"/>
       <c r="I1865" s="53"/>
@@ -26375,7 +26696,9 @@
       <c r="E1866" s="3" t="s">
         <v>4290</v>
       </c>
-      <c r="F1866" s="3"/>
+      <c r="F1866" s="81" t="s">
+        <v>4481</v>
+      </c>
       <c r="G1866" s="3"/>
       <c r="H1866" s="3"/>
       <c r="I1866" s="53"/>
@@ -26413,7 +26736,7 @@
       <c r="C1867" s="62"/>
       <c r="D1867" s="3"/>
       <c r="E1867" s="3"/>
-      <c r="F1867" s="3"/>
+      <c r="F1867" s="81"/>
       <c r="G1867" s="3"/>
       <c r="H1867" s="3"/>
       <c r="I1867" s="53"/>
@@ -26443,7 +26766,7 @@
       <c r="C1868" s="62"/>
       <c r="D1868" s="3"/>
       <c r="E1868" s="3"/>
-      <c r="F1868" s="3"/>
+      <c r="F1868" s="81"/>
       <c r="G1868" s="3"/>
       <c r="H1868" s="3"/>
       <c r="I1868" s="53"/>
@@ -26503,7 +26826,7 @@
       </c>
       <c r="D1870" s="5"/>
       <c r="E1870" s="46"/>
-      <c r="F1870" s="46"/>
+      <c r="F1870" s="82"/>
       <c r="G1870" s="46"/>
       <c r="H1870" s="46"/>
       <c r="I1870" s="46"/>
@@ -26529,7 +26852,7 @@
       <c r="C1871" s="62"/>
       <c r="D1871" s="3"/>
       <c r="E1871" s="53"/>
-      <c r="F1871" s="53"/>
+      <c r="F1871" s="81"/>
       <c r="G1871" s="53"/>
       <c r="H1871" s="53"/>
       <c r="I1871" s="53"/>
@@ -26551,7 +26874,7 @@
       <c r="C1872" s="62"/>
       <c r="D1872" s="3"/>
       <c r="E1872" s="53"/>
-      <c r="F1872" s="53"/>
+      <c r="F1872" s="81"/>
       <c r="G1872" s="53"/>
       <c r="H1872" s="53"/>
       <c r="I1872" s="53"/>
@@ -26573,7 +26896,7 @@
       <c r="C1873" s="64"/>
       <c r="D1873" s="30"/>
       <c r="E1873" s="65"/>
-      <c r="F1873" s="65"/>
+      <c r="F1873" s="83"/>
       <c r="G1873" s="65"/>
       <c r="H1873" s="65"/>
       <c r="I1873" s="65"/>
@@ -26601,7 +26924,7 @@
         <v>4358</v>
       </c>
       <c r="E1874" s="46"/>
-      <c r="F1874" s="46"/>
+      <c r="F1874" s="82"/>
       <c r="G1874" s="46" t="s">
         <v>4340</v>
       </c>
@@ -26626,7 +26949,7 @@
       <c r="C1875" s="62"/>
       <c r="D1875" s="3"/>
       <c r="E1875" s="53"/>
-      <c r="F1875" s="53"/>
+      <c r="F1875" s="81"/>
       <c r="G1875" s="53"/>
       <c r="H1875" s="53"/>
       <c r="I1875" s="53"/>
@@ -26651,7 +26974,7 @@
       <c r="C1876" s="62"/>
       <c r="D1876" s="3"/>
       <c r="E1876" s="53"/>
-      <c r="F1876" s="53"/>
+      <c r="F1876" s="81"/>
       <c r="G1876" s="53"/>
       <c r="H1876" s="53"/>
       <c r="I1876" s="53"/>
@@ -26673,7 +26996,7 @@
       <c r="C1877" s="62"/>
       <c r="D1877" s="3"/>
       <c r="E1877" s="53"/>
-      <c r="F1877" s="53"/>
+      <c r="F1877" s="81"/>
       <c r="G1877" s="53"/>
       <c r="H1877" s="53"/>
       <c r="I1877" s="53"/>
@@ -26696,7 +27019,7 @@
       <c r="C1878" s="62"/>
       <c r="D1878" s="3"/>
       <c r="E1878" s="53"/>
-      <c r="F1878" s="53"/>
+      <c r="F1878" s="81"/>
       <c r="G1878" s="53"/>
       <c r="H1878" s="53"/>
       <c r="I1878" s="53"/>
@@ -26719,7 +27042,7 @@
       <c r="C1879" s="62"/>
       <c r="D1879" s="3"/>
       <c r="E1879" s="53"/>
-      <c r="F1879" s="53"/>
+      <c r="F1879" s="81"/>
       <c r="G1879" s="53"/>
       <c r="H1879" s="53"/>
       <c r="I1879" s="53"/>
@@ -26742,7 +27065,7 @@
       <c r="C1880" s="62"/>
       <c r="D1880" s="3"/>
       <c r="E1880" s="53"/>
-      <c r="F1880" s="53"/>
+      <c r="F1880" s="81"/>
       <c r="G1880" s="53"/>
       <c r="H1880" s="53"/>
       <c r="I1880" s="53"/>
@@ -26757,7 +27080,7 @@
       <c r="R1880" s="42"/>
       <c r="S1880" s="42"/>
     </row>
-    <row r="1881" spans="1:19">
+    <row r="1881" spans="1:19" ht="27.000000">
       <c r="A1881" s="58" t="s">
         <v>27</v>
       </c>
@@ -26765,7 +27088,7 @@
       <c r="C1881" s="62"/>
       <c r="D1881" s="3"/>
       <c r="E1881" s="53"/>
-      <c r="F1881" s="53" t="s">
+      <c r="F1881" s="81" t="s">
         <v>4347</v>
       </c>
       <c r="G1881" s="53"/>
@@ -26819,7 +27142,7 @@
       <c r="C1883" s="62"/>
       <c r="D1883" s="3"/>
       <c r="E1883" s="53"/>
-      <c r="F1883" s="53"/>
+      <c r="F1883" s="81"/>
       <c r="G1883" s="53"/>
       <c r="H1883" s="53"/>
       <c r="I1883" s="53"/>
@@ -26842,7 +27165,7 @@
       <c r="C1884" s="62"/>
       <c r="D1884" s="3"/>
       <c r="E1884" s="53"/>
-      <c r="F1884" s="53"/>
+      <c r="F1884" s="81"/>
       <c r="G1884" s="53"/>
       <c r="H1884" s="53"/>
       <c r="I1884" s="53"/>
@@ -26865,7 +27188,7 @@
       <c r="C1885" s="62"/>
       <c r="D1885" s="3"/>
       <c r="E1885" s="53"/>
-      <c r="F1885" s="53"/>
+      <c r="F1885" s="81"/>
       <c r="G1885" s="53"/>
       <c r="H1885" s="53"/>
       <c r="I1885" s="53"/>
@@ -26888,7 +27211,7 @@
       <c r="C1886" s="62"/>
       <c r="D1886" s="3"/>
       <c r="E1886" s="53"/>
-      <c r="F1886" s="53"/>
+      <c r="F1886" s="81"/>
       <c r="G1886" s="53"/>
       <c r="H1886" s="53"/>
       <c r="I1886" s="53"/>
@@ -26911,7 +27234,7 @@
       <c r="C1887" s="62"/>
       <c r="D1887" s="3"/>
       <c r="E1887" s="53"/>
-      <c r="F1887" s="53"/>
+      <c r="F1887" s="81"/>
       <c r="G1887" s="53"/>
       <c r="H1887" s="53"/>
       <c r="I1887" s="53"/>
@@ -26934,7 +27257,7 @@
       <c r="C1888" s="62"/>
       <c r="D1888" s="3"/>
       <c r="E1888" s="53"/>
-      <c r="F1888" s="53"/>
+      <c r="F1888" s="81"/>
       <c r="G1888" s="53"/>
       <c r="H1888" s="53"/>
       <c r="I1888" s="53"/>
@@ -26957,7 +27280,7 @@
       <c r="C1889" s="62"/>
       <c r="D1889" s="3"/>
       <c r="E1889" s="53"/>
-      <c r="F1889" s="53"/>
+      <c r="F1889" s="81"/>
       <c r="G1889" s="53"/>
       <c r="H1889" s="53"/>
       <c r="I1889" s="53"/>
@@ -26982,7 +27305,7 @@
         <v>4405</v>
       </c>
       <c r="E1890" s="53"/>
-      <c r="F1890" s="53"/>
+      <c r="F1890" s="81"/>
       <c r="G1890" s="53"/>
       <c r="H1890" s="53"/>
       <c r="I1890" s="53"/>
@@ -27003,7 +27326,7 @@
       <c r="C1891" s="62"/>
       <c r="D1891" s="55"/>
       <c r="E1891" s="53"/>
-      <c r="F1891" s="53"/>
+      <c r="F1891" s="81"/>
       <c r="G1891" s="53"/>
       <c r="H1891" s="53"/>
       <c r="I1891" s="53"/>
@@ -27026,7 +27349,7 @@
       <c r="C1892" s="62"/>
       <c r="D1892" s="55"/>
       <c r="E1892" s="53"/>
-      <c r="F1892" s="53"/>
+      <c r="F1892" s="81"/>
       <c r="G1892" s="53"/>
       <c r="H1892" s="53"/>
       <c r="I1892" s="53"/>
@@ -27049,7 +27372,7 @@
       <c r="C1893" s="62"/>
       <c r="D1893" s="55"/>
       <c r="E1893" s="53"/>
-      <c r="F1893" s="53"/>
+      <c r="F1893" s="81"/>
       <c r="G1893" s="53"/>
       <c r="H1893" s="53"/>
       <c r="I1893" s="53"/>
@@ -27072,7 +27395,7 @@
       <c r="C1894" s="62"/>
       <c r="D1894" s="55"/>
       <c r="E1894" s="53"/>
-      <c r="F1894" s="53"/>
+      <c r="F1894" s="81"/>
       <c r="G1894" s="53"/>
       <c r="H1894" s="53"/>
       <c r="I1894" s="53"/>
@@ -27097,7 +27420,7 @@
         <v>4406</v>
       </c>
       <c r="E1895" s="53"/>
-      <c r="F1895" s="53"/>
+      <c r="F1895" s="81"/>
       <c r="G1895" s="53"/>
       <c r="H1895" s="53"/>
       <c r="I1895" s="53"/>
@@ -27120,7 +27443,7 @@
       <c r="C1896" s="62"/>
       <c r="D1896" s="55"/>
       <c r="E1896" s="53"/>
-      <c r="F1896" s="53"/>
+      <c r="F1896" s="81"/>
       <c r="G1896" s="53"/>
       <c r="H1896" s="53"/>
       <c r="I1896" s="53"/>
@@ -27143,7 +27466,7 @@
       <c r="C1897" s="62"/>
       <c r="D1897" s="55"/>
       <c r="E1897" s="53"/>
-      <c r="F1897" s="53"/>
+      <c r="F1897" s="81"/>
       <c r="G1897" s="53"/>
       <c r="H1897" s="53"/>
       <c r="I1897" s="53"/>
@@ -27166,7 +27489,7 @@
       <c r="C1898" s="62"/>
       <c r="D1898" s="55"/>
       <c r="E1898" s="53"/>
-      <c r="F1898" s="53"/>
+      <c r="F1898" s="81"/>
       <c r="G1898" s="53"/>
       <c r="H1898" s="53"/>
       <c r="I1898" s="53"/>
@@ -27181,7 +27504,7 @@
       <c r="R1898" s="42"/>
       <c r="S1898" s="42"/>
     </row>
-    <row r="1899" spans="1:19" ht="27.000000">
+    <row r="1899" spans="1:19" ht="40.500000">
       <c r="A1899" s="58" t="s">
         <v>42</v>
       </c>
@@ -27189,7 +27512,7 @@
       <c r="C1899" s="62"/>
       <c r="D1899" s="55"/>
       <c r="E1899" s="53"/>
-      <c r="F1899" s="53"/>
+      <c r="F1899" s="81"/>
       <c r="G1899" s="53"/>
       <c r="H1899" s="53"/>
       <c r="I1899" s="53"/>
@@ -27243,7 +27566,7 @@
       <c r="C1901" s="62"/>
       <c r="D1901" s="55"/>
       <c r="E1901" s="53"/>
-      <c r="F1901" s="53" t="s">
+      <c r="F1901" s="81" t="s">
         <v>4415</v>
       </c>
       <c r="G1901" s="53"/>
@@ -27270,7 +27593,7 @@
       <c r="C1902" s="62"/>
       <c r="D1902" s="55"/>
       <c r="E1902" s="53"/>
-      <c r="F1902" s="53" t="s">
+      <c r="F1902" s="81" t="s">
         <v>4433</v>
       </c>
       <c r="G1902" s="53"/>
@@ -27295,7 +27618,7 @@
       <c r="C1903" s="62"/>
       <c r="D1903" s="55"/>
       <c r="E1903" s="53"/>
-      <c r="F1903" s="53" t="s">
+      <c r="F1903" s="81" t="s">
         <v>4418</v>
       </c>
       <c r="G1903" s="53"/>
@@ -27322,7 +27645,7 @@
       <c r="C1904" s="62"/>
       <c r="D1904" s="55"/>
       <c r="E1904" s="53"/>
-      <c r="F1904" s="53"/>
+      <c r="F1904" s="81"/>
       <c r="G1904" s="53"/>
       <c r="H1904" s="53"/>
       <c r="I1904" s="53"/>
@@ -27345,7 +27668,7 @@
       <c r="C1905" s="62"/>
       <c r="D1905" s="55"/>
       <c r="E1905" s="53"/>
-      <c r="F1905" s="53"/>
+      <c r="F1905" s="81"/>
       <c r="G1905" s="53"/>
       <c r="H1905" s="53"/>
       <c r="I1905" s="53" t="s">
@@ -27370,7 +27693,7 @@
       <c r="C1906" s="62"/>
       <c r="D1906" s="55"/>
       <c r="E1906" s="53"/>
-      <c r="F1906" s="53" t="s">
+      <c r="F1906" s="81" t="s">
         <v>4441</v>
       </c>
       <c r="G1906" s="53" t="s">
@@ -27397,7 +27720,7 @@
       <c r="C1907" s="62"/>
       <c r="D1907" s="55"/>
       <c r="E1907" s="53"/>
-      <c r="F1907" s="53"/>
+      <c r="F1907" s="81"/>
       <c r="G1907" s="53"/>
       <c r="H1907" s="53"/>
       <c r="I1907" s="53"/>
@@ -27420,7 +27743,7 @@
       <c r="C1908" s="62"/>
       <c r="D1908" s="55"/>
       <c r="E1908" s="53"/>
-      <c r="F1908" s="53"/>
+      <c r="F1908" s="81"/>
       <c r="G1908" s="53"/>
       <c r="H1908" s="53"/>
       <c r="I1908" s="53"/>
@@ -27443,7 +27766,7 @@
       <c r="C1909" s="62"/>
       <c r="D1909" s="55"/>
       <c r="E1909" s="53"/>
-      <c r="F1909" s="53"/>
+      <c r="F1909" s="81"/>
       <c r="G1909" s="53"/>
       <c r="H1909" s="53"/>
       <c r="I1909" s="53"/>
@@ -27466,7 +27789,7 @@
       <c r="C1910" s="62"/>
       <c r="D1910" s="55"/>
       <c r="E1910" s="53"/>
-      <c r="F1910" s="53"/>
+      <c r="F1910" s="81"/>
       <c r="G1910" s="53"/>
       <c r="H1910" s="53"/>
       <c r="I1910" s="53"/>
@@ -27489,7 +27812,7 @@
       <c r="C1911" s="62"/>
       <c r="D1911" s="55"/>
       <c r="E1911" s="53"/>
-      <c r="F1911" s="53"/>
+      <c r="F1911" s="81"/>
       <c r="G1911" s="53"/>
       <c r="H1911" s="53"/>
       <c r="I1911" s="53"/>
@@ -27514,7 +27837,7 @@
       <c r="C1912" s="62"/>
       <c r="D1912" s="55"/>
       <c r="E1912" s="53"/>
-      <c r="F1912" s="53" t="s">
+      <c r="F1912" s="81" t="s">
         <v>4447</v>
       </c>
       <c r="G1912" s="53"/>
@@ -27541,7 +27864,7 @@
       <c r="C1913" s="62"/>
       <c r="D1913" s="55"/>
       <c r="E1913" s="53"/>
-      <c r="F1913" s="53"/>
+      <c r="F1913" s="81"/>
       <c r="G1913" s="53"/>
       <c r="H1913" s="53"/>
       <c r="I1913" s="53"/>
@@ -27564,7 +27887,7 @@
       <c r="C1914" s="62"/>
       <c r="D1914" s="55"/>
       <c r="E1914" s="53"/>
-      <c r="F1914" s="53"/>
+      <c r="F1914" s="81"/>
       <c r="G1914" s="53"/>
       <c r="H1914" s="53"/>
       <c r="I1914" s="53"/>
@@ -27589,7 +27912,7 @@
       <c r="C1915" s="62"/>
       <c r="D1915" s="55"/>
       <c r="E1915" s="53"/>
-      <c r="F1915" s="53"/>
+      <c r="F1915" s="81"/>
       <c r="G1915" s="53"/>
       <c r="H1915" s="53"/>
       <c r="I1915" s="53"/>
@@ -27612,7 +27935,7 @@
       <c r="C1916" s="62"/>
       <c r="D1916" s="55"/>
       <c r="E1916" s="53"/>
-      <c r="F1916" s="53" t="s">
+      <c r="F1916" s="81" t="s">
         <v>4422</v>
       </c>
       <c r="G1916" s="53"/>
@@ -27637,7 +27960,7 @@
       <c r="C1917" s="62"/>
       <c r="D1917" s="55"/>
       <c r="E1917" s="53"/>
-      <c r="F1917" s="53"/>
+      <c r="F1917" s="81"/>
       <c r="G1917" s="53"/>
       <c r="H1917" s="53"/>
       <c r="I1917" s="53"/>
@@ -27660,7 +27983,7 @@
       <c r="C1918" s="62"/>
       <c r="D1918" s="55"/>
       <c r="E1918" s="53"/>
-      <c r="F1918" s="53"/>
+      <c r="F1918" s="81"/>
       <c r="G1918" s="53"/>
       <c r="H1918" s="53"/>
       <c r="I1918" s="53"/>
@@ -27683,7 +28006,7 @@
       <c r="C1919" s="62"/>
       <c r="D1919" s="55"/>
       <c r="E1919" s="53"/>
-      <c r="F1919" s="53"/>
+      <c r="F1919" s="81"/>
       <c r="G1919" s="53"/>
       <c r="H1919" s="53"/>
       <c r="I1919" s="53"/>
@@ -27706,7 +28029,7 @@
       <c r="C1920" s="62"/>
       <c r="D1920" s="55"/>
       <c r="E1920" s="53"/>
-      <c r="F1920" s="53" t="s">
+      <c r="F1920" s="81" t="s">
         <v>4445</v>
       </c>
       <c r="G1920" s="53"/>
@@ -27731,7 +28054,7 @@
       <c r="C1921" s="62"/>
       <c r="D1921" s="55"/>
       <c r="E1921" s="53"/>
-      <c r="F1921" s="53"/>
+      <c r="F1921" s="81"/>
       <c r="G1921" s="53"/>
       <c r="H1921" s="53"/>
       <c r="I1921" s="53"/>
@@ -27754,7 +28077,7 @@
       <c r="C1922" s="62"/>
       <c r="D1922" s="55"/>
       <c r="E1922" s="53"/>
-      <c r="F1922" s="53" t="s">
+      <c r="F1922" s="81" t="s">
         <v>4446</v>
       </c>
       <c r="G1922" s="53"/>
@@ -27771,7 +28094,7 @@
       <c r="R1922" s="42"/>
       <c r="S1922" s="42"/>
     </row>
-    <row r="1923" spans="1:19">
+    <row r="1923" spans="1:19" ht="27.000000">
       <c r="A1923" s="58" t="s">
         <v>65</v>
       </c>
@@ -27779,7 +28102,7 @@
       <c r="C1923" s="62"/>
       <c r="D1923" s="55"/>
       <c r="E1923" s="53"/>
-      <c r="F1923" s="53"/>
+      <c r="F1923" s="81"/>
       <c r="G1923" s="53"/>
       <c r="H1923" s="53"/>
       <c r="I1923" s="53"/>
@@ -27833,7 +28156,7 @@
       <c r="C1925" s="62"/>
       <c r="D1925" s="55"/>
       <c r="E1925" s="53"/>
-      <c r="F1925" s="53" t="s">
+      <c r="F1925" s="81" t="s">
         <v>4458</v>
       </c>
       <c r="G1925" s="53"/>
@@ -27858,7 +28181,7 @@
       <c r="C1926" s="62"/>
       <c r="D1926" s="55"/>
       <c r="E1926" s="53"/>
-      <c r="F1926" s="53"/>
+      <c r="F1926" s="81"/>
       <c r="G1926" s="53"/>
       <c r="H1926" s="53"/>
       <c r="I1926" s="53"/>
@@ -27881,7 +28204,7 @@
       <c r="C1927" s="62"/>
       <c r="D1927" s="55"/>
       <c r="E1927" s="53"/>
-      <c r="F1927" s="53" t="s">
+      <c r="F1927" s="81" t="s">
         <v>4453</v>
       </c>
       <c r="G1927" s="53"/>
@@ -27906,7 +28229,7 @@
       <c r="C1928" s="62"/>
       <c r="D1928" s="55"/>
       <c r="E1928" s="53"/>
-      <c r="F1928" s="53"/>
+      <c r="F1928" s="81"/>
       <c r="G1928" s="53"/>
       <c r="H1928" s="53"/>
       <c r="I1928" s="53"/>
@@ -27929,7 +28252,7 @@
       <c r="C1929" s="62"/>
       <c r="D1929" s="55"/>
       <c r="E1929" s="53"/>
-      <c r="F1929" s="53"/>
+      <c r="F1929" s="81"/>
       <c r="G1929" s="53"/>
       <c r="H1929" s="53"/>
       <c r="I1929" s="53"/>
@@ -27952,7 +28275,7 @@
       <c r="C1930" s="62"/>
       <c r="D1930" s="55"/>
       <c r="E1930" s="53"/>
-      <c r="F1930" s="53"/>
+      <c r="F1930" s="81"/>
       <c r="G1930" s="53"/>
       <c r="H1930" s="53"/>
       <c r="I1930" s="53"/>
@@ -27977,7 +28300,7 @@
       <c r="C1931" s="62"/>
       <c r="D1931" s="55"/>
       <c r="E1931" s="53"/>
-      <c r="F1931" s="53"/>
+      <c r="F1931" s="81"/>
       <c r="G1931" s="53"/>
       <c r="H1931" s="53"/>
       <c r="I1931" s="53" t="s">
@@ -28002,7 +28325,7 @@
       <c r="C1932" s="62"/>
       <c r="D1932" s="55"/>
       <c r="E1932" s="53"/>
-      <c r="F1932" s="53"/>
+      <c r="F1932" s="81"/>
       <c r="G1932" s="53"/>
       <c r="H1932" s="53"/>
       <c r="I1932" s="53"/>
@@ -28025,7 +28348,7 @@
       <c r="C1933" s="62"/>
       <c r="D1933" s="55"/>
       <c r="E1933" s="53"/>
-      <c r="F1933" s="53"/>
+      <c r="F1933" s="81"/>
       <c r="G1933" s="53"/>
       <c r="H1933" s="53"/>
       <c r="I1933" s="53"/>
@@ -28048,7 +28371,7 @@
       <c r="C1934" s="62"/>
       <c r="D1934" s="55"/>
       <c r="E1934" s="53"/>
-      <c r="F1934" s="53"/>
+      <c r="F1934" s="81"/>
       <c r="G1934" s="53"/>
       <c r="H1934" s="53"/>
       <c r="I1934" s="53"/>
@@ -28071,7 +28394,7 @@
       <c r="C1935" s="62"/>
       <c r="D1935" s="55"/>
       <c r="E1935" s="53"/>
-      <c r="F1935" s="53"/>
+      <c r="F1935" s="81"/>
       <c r="G1935" s="53"/>
       <c r="H1935" s="53"/>
       <c r="I1935" s="53"/>
@@ -28094,7 +28417,7 @@
       <c r="C1936" s="62"/>
       <c r="D1936" s="55"/>
       <c r="E1936" s="53"/>
-      <c r="F1936" s="53"/>
+      <c r="F1936" s="81"/>
       <c r="G1936" s="53"/>
       <c r="H1936" s="53"/>
       <c r="I1936" s="53"/>
@@ -28117,7 +28440,7 @@
       <c r="C1937" s="62"/>
       <c r="D1937" s="55"/>
       <c r="E1937" s="53"/>
-      <c r="F1937" s="53"/>
+      <c r="F1937" s="81"/>
       <c r="G1937" s="53"/>
       <c r="H1937" s="53"/>
       <c r="I1937" s="53"/>
@@ -28140,7 +28463,7 @@
       <c r="C1938" s="62"/>
       <c r="D1938" s="55"/>
       <c r="E1938" s="53"/>
-      <c r="F1938" s="53"/>
+      <c r="F1938" s="81"/>
       <c r="G1938" s="53"/>
       <c r="H1938" s="53"/>
       <c r="I1938" s="53"/>
@@ -28163,7 +28486,7 @@
       <c r="C1939" s="62"/>
       <c r="D1939" s="55"/>
       <c r="E1939" s="53"/>
-      <c r="F1939" s="53"/>
+      <c r="F1939" s="81"/>
       <c r="G1939" s="53"/>
       <c r="H1939" s="53"/>
       <c r="I1939" s="53"/>
@@ -28186,7 +28509,7 @@
       <c r="C1940" s="62"/>
       <c r="D1940" s="55"/>
       <c r="E1940" s="53"/>
-      <c r="F1940" s="53" t="s">
+      <c r="F1940" s="81" t="s">
         <v>4456</v>
       </c>
       <c r="G1940" s="53"/>
@@ -28234,7 +28557,7 @@
       <c r="P1941" s="53"/>
       <c r="Q1941" s="66"/>
     </row>
-    <row r="1942" spans="1:19">
+    <row r="1942" spans="1:19" ht="40.500000">
       <c r="A1942" s="58" t="s">
         <v>82</v>
       </c>
@@ -28244,7 +28567,7 @@
       <c r="E1942" s="3" t="s">
         <v>4468</v>
       </c>
-      <c r="F1942" s="53"/>
+      <c r="F1942" s="81"/>
       <c r="G1942" s="53"/>
       <c r="H1942" s="53"/>
       <c r="I1942" s="53"/>
@@ -28253,7 +28576,9 @@
       <c r="L1942" s="53"/>
       <c r="M1942" s="53"/>
       <c r="N1942" s="53"/>
-      <c r="O1942" s="53"/>
+      <c r="O1942" s="53" t="s">
+        <v>4489</v>
+      </c>
       <c r="P1942" s="53"/>
       <c r="Q1942" s="66"/>
       <c r="R1942" s="42"/>
@@ -28267,7 +28592,7 @@
       <c r="C1943" s="62"/>
       <c r="D1943" s="55"/>
       <c r="E1943" s="3"/>
-      <c r="F1943" s="53"/>
+      <c r="F1943" s="81"/>
       <c r="G1943" s="53"/>
       <c r="H1943" s="53"/>
       <c r="I1943" s="53"/>
@@ -28290,7 +28615,7 @@
       <c r="C1944" s="62"/>
       <c r="D1944" s="55"/>
       <c r="E1944" s="3"/>
-      <c r="F1944" s="53"/>
+      <c r="F1944" s="81"/>
       <c r="G1944" s="53"/>
       <c r="H1944" s="53"/>
       <c r="I1944" s="53"/>
@@ -28313,7 +28638,7 @@
       <c r="C1945" s="62"/>
       <c r="D1945" s="55"/>
       <c r="E1945" s="3"/>
-      <c r="F1945" s="53"/>
+      <c r="F1945" s="81"/>
       <c r="G1945" s="53"/>
       <c r="H1945" s="53"/>
       <c r="I1945" s="53"/>
@@ -28336,7 +28661,7 @@
       <c r="C1946" s="62"/>
       <c r="D1946" s="55"/>
       <c r="E1946" s="3"/>
-      <c r="F1946" s="53"/>
+      <c r="F1946" s="81"/>
       <c r="G1946" s="53"/>
       <c r="H1946" s="53"/>
       <c r="I1946" s="53"/>
@@ -28359,7 +28684,7 @@
       <c r="C1947" s="62"/>
       <c r="D1947" s="55"/>
       <c r="E1947" s="3"/>
-      <c r="F1947" s="53" t="s">
+      <c r="F1947" s="81" t="s">
         <v>4459</v>
       </c>
       <c r="G1947" s="53"/>
@@ -28376,7 +28701,7 @@
       <c r="R1947" s="42"/>
       <c r="S1947" s="42"/>
     </row>
-    <row r="1948" spans="1:19">
+    <row r="1948" spans="1:19" ht="27.000000">
       <c r="A1948" s="58" t="s">
         <v>88</v>
       </c>
@@ -28386,7 +28711,9 @@
       <c r="E1948" s="3" t="s">
         <v>4469</v>
       </c>
-      <c r="F1948" s="53"/>
+      <c r="F1948" s="81" t="s">
+        <v>4484</v>
+      </c>
       <c r="G1948" s="53"/>
       <c r="H1948" s="53"/>
       <c r="I1948" s="53"/>
@@ -28409,7 +28736,7 @@
       <c r="C1949" s="62"/>
       <c r="D1949" s="55"/>
       <c r="E1949" s="3"/>
-      <c r="F1949" s="53"/>
+      <c r="F1949" s="81"/>
       <c r="G1949" s="53"/>
       <c r="H1949" s="53"/>
       <c r="I1949" s="53"/>
@@ -28424,7 +28751,7 @@
       <c r="R1949" s="42"/>
       <c r="S1949" s="42"/>
     </row>
-    <row r="1950" spans="1:19">
+    <row r="1950" spans="1:19" ht="27.000000">
       <c r="A1950" s="58" t="s">
         <v>90</v>
       </c>
@@ -28432,7 +28759,9 @@
       <c r="C1950" s="62"/>
       <c r="D1950" s="55"/>
       <c r="E1950" s="3"/>
-      <c r="F1950" s="53"/>
+      <c r="F1950" s="81" t="s">
+        <v>4546</v>
+      </c>
       <c r="G1950" s="53"/>
       <c r="H1950" s="53"/>
       <c r="I1950" s="53"/>
@@ -28455,7 +28784,7 @@
       <c r="C1951" s="62"/>
       <c r="D1951" s="55"/>
       <c r="E1951" s="3"/>
-      <c r="F1951" s="53"/>
+      <c r="F1951" s="81"/>
       <c r="G1951" s="53"/>
       <c r="H1951" s="53"/>
       <c r="I1951" s="53"/>
@@ -28478,7 +28807,9 @@
       <c r="C1952" s="62"/>
       <c r="D1952" s="55"/>
       <c r="E1952" s="3"/>
-      <c r="F1952" s="53"/>
+      <c r="F1952" s="81" t="s">
+        <v>4491</v>
+      </c>
       <c r="G1952" s="53"/>
       <c r="H1952" s="53"/>
       <c r="I1952" s="53"/>
@@ -28501,7 +28832,9 @@
       <c r="C1953" s="62"/>
       <c r="D1953" s="55"/>
       <c r="E1953" s="3"/>
-      <c r="F1953" s="53"/>
+      <c r="F1953" s="81" t="s">
+        <v>4490</v>
+      </c>
       <c r="G1953" s="53"/>
       <c r="H1953" s="53"/>
       <c r="I1953" s="53"/>
@@ -28526,7 +28859,7 @@
       <c r="E1954" s="3" t="s">
         <v>4470</v>
       </c>
-      <c r="F1954" s="53"/>
+      <c r="F1954" s="81"/>
       <c r="G1954" s="53"/>
       <c r="H1954" s="53"/>
       <c r="I1954" s="53"/>
@@ -28541,7 +28874,7 @@
       <c r="R1954" s="42"/>
       <c r="S1954" s="42"/>
     </row>
-    <row r="1955" spans="1:19">
+    <row r="1955" spans="1:19" ht="54.000000">
       <c r="A1955" s="58" t="s">
         <v>95</v>
       </c>
@@ -28549,7 +28882,9 @@
       <c r="C1955" s="62"/>
       <c r="D1955" s="55"/>
       <c r="E1955" s="3"/>
-      <c r="F1955" s="53"/>
+      <c r="F1955" s="81" t="s">
+        <v>4496</v>
+      </c>
       <c r="G1955" s="53"/>
       <c r="H1955" s="53"/>
       <c r="I1955" s="53"/>
@@ -28572,7 +28907,7 @@
       <c r="C1956" s="62"/>
       <c r="D1956" s="55"/>
       <c r="E1956" s="3"/>
-      <c r="F1956" s="53"/>
+      <c r="F1956" s="81"/>
       <c r="G1956" s="53"/>
       <c r="H1956" s="53"/>
       <c r="I1956" s="53"/>
@@ -28595,7 +28930,7 @@
       <c r="C1957" s="62"/>
       <c r="D1957" s="55"/>
       <c r="E1957" s="3"/>
-      <c r="F1957" s="53"/>
+      <c r="F1957" s="81"/>
       <c r="G1957" s="53"/>
       <c r="H1957" s="53"/>
       <c r="I1957" s="53"/>
@@ -28618,7 +28953,7 @@
       <c r="C1958" s="62"/>
       <c r="D1958" s="55"/>
       <c r="E1958" s="3"/>
-      <c r="F1958" s="53"/>
+      <c r="F1958" s="81"/>
       <c r="G1958" s="53"/>
       <c r="H1958" s="53"/>
       <c r="I1958" s="53"/>
@@ -28641,7 +28976,9 @@
       <c r="C1959" s="62"/>
       <c r="D1959" s="55"/>
       <c r="E1959" s="3"/>
-      <c r="F1959" s="53"/>
+      <c r="F1959" s="81" t="s">
+        <v>4497</v>
+      </c>
       <c r="G1959" s="53"/>
       <c r="H1959" s="53"/>
       <c r="I1959" s="53"/>
@@ -28656,7 +28993,7 @@
       <c r="R1959" s="42"/>
       <c r="S1959" s="42"/>
     </row>
-    <row r="1960" spans="1:19">
+    <row r="1960" spans="1:19" ht="27.000000">
       <c r="A1960" s="58" t="s">
         <v>100</v>
       </c>
@@ -28666,7 +29003,9 @@
       <c r="E1960" s="3" t="s">
         <v>4471</v>
       </c>
-      <c r="F1960" s="53"/>
+      <c r="F1960" s="81" t="s">
+        <v>4498</v>
+      </c>
       <c r="G1960" s="53"/>
       <c r="H1960" s="53"/>
       <c r="I1960" s="53"/>
@@ -28681,7 +29020,7 @@
       <c r="R1960" s="42"/>
       <c r="S1960" s="42"/>
     </row>
-    <row r="1961" spans="1:19">
+    <row r="1961" spans="1:19" ht="27.000000">
       <c r="A1961" s="58" t="s">
         <v>101</v>
       </c>
@@ -28689,7 +29028,9 @@
       <c r="C1961" s="62"/>
       <c r="D1961" s="55"/>
       <c r="E1961" s="3"/>
-      <c r="F1961" s="53"/>
+      <c r="F1961" s="81" t="s">
+        <v>4500</v>
+      </c>
       <c r="G1961" s="53"/>
       <c r="H1961" s="53"/>
       <c r="I1961" s="53"/>
@@ -28712,7 +29053,7 @@
       <c r="C1962" s="62"/>
       <c r="D1962" s="55"/>
       <c r="E1962" s="3"/>
-      <c r="F1962" s="53"/>
+      <c r="F1962" s="81"/>
       <c r="G1962" s="53"/>
       <c r="H1962" s="53"/>
       <c r="I1962" s="53"/>
@@ -28727,7 +29068,7 @@
       <c r="R1962" s="42"/>
       <c r="S1962" s="42"/>
     </row>
-    <row r="1963" spans="1:19">
+    <row r="1963" spans="1:19" ht="27.000000">
       <c r="A1963" s="58" t="s">
         <v>103</v>
       </c>
@@ -28735,7 +29076,9 @@
       <c r="C1963" s="62"/>
       <c r="D1963" s="55"/>
       <c r="E1963" s="3"/>
-      <c r="F1963" s="53"/>
+      <c r="F1963" s="81" t="s">
+        <v>4501</v>
+      </c>
       <c r="G1963" s="53"/>
       <c r="H1963" s="53"/>
       <c r="I1963" s="53"/>
@@ -28758,7 +29101,7 @@
       <c r="C1964" s="62"/>
       <c r="D1964" s="55"/>
       <c r="E1964" s="3"/>
-      <c r="F1964" s="53"/>
+      <c r="F1964" s="81"/>
       <c r="G1964" s="53"/>
       <c r="H1964" s="53"/>
       <c r="I1964" s="53"/>
@@ -28781,7 +29124,9 @@
       <c r="C1965" s="62"/>
       <c r="D1965" s="55"/>
       <c r="E1965" s="3"/>
-      <c r="F1965" s="53"/>
+      <c r="F1965" s="81" t="s">
+        <v>4502</v>
+      </c>
       <c r="G1965" s="53"/>
       <c r="H1965" s="53"/>
       <c r="I1965" s="53"/>
@@ -28806,7 +29151,7 @@
       <c r="E1966" s="3" t="s">
         <v>4474</v>
       </c>
-      <c r="F1966" s="53"/>
+      <c r="F1966" s="81"/>
       <c r="G1966" s="53"/>
       <c r="H1966" s="53"/>
       <c r="I1966" s="53"/>
@@ -28829,7 +29174,9 @@
       <c r="C1967" s="62"/>
       <c r="D1967" s="55"/>
       <c r="E1967" s="3"/>
-      <c r="F1967" s="53"/>
+      <c r="F1967" s="81" t="s">
+        <v>4503</v>
+      </c>
       <c r="G1967" s="53"/>
       <c r="H1967" s="53"/>
       <c r="I1967" s="53"/>
@@ -28852,7 +29199,9 @@
       <c r="C1968" s="62"/>
       <c r="D1968" s="55"/>
       <c r="E1968" s="3"/>
-      <c r="F1968" s="53"/>
+      <c r="F1968" s="81" t="s">
+        <v>4504</v>
+      </c>
       <c r="G1968" s="53"/>
       <c r="H1968" s="53"/>
       <c r="I1968" s="53"/>
@@ -28875,7 +29224,7 @@
       <c r="C1969" s="62"/>
       <c r="D1969" s="55"/>
       <c r="E1969" s="3"/>
-      <c r="F1969" s="53"/>
+      <c r="F1969" s="81"/>
       <c r="G1969" s="53"/>
       <c r="H1969" s="53"/>
       <c r="I1969" s="53"/>
@@ -28898,7 +29247,7 @@
       <c r="C1970" s="62"/>
       <c r="D1970" s="55"/>
       <c r="E1970" s="3"/>
-      <c r="F1970" s="53"/>
+      <c r="F1970" s="81"/>
       <c r="G1970" s="53"/>
       <c r="H1970" s="53"/>
       <c r="I1970" s="53"/>
@@ -28921,7 +29270,7 @@
       <c r="C1971" s="62"/>
       <c r="D1971" s="55"/>
       <c r="E1971" s="3"/>
-      <c r="F1971" s="53"/>
+      <c r="F1971" s="81"/>
       <c r="G1971" s="53"/>
       <c r="H1971" s="53"/>
       <c r="I1971" s="53"/>
@@ -28946,7 +29295,7 @@
       <c r="E1972" s="3" t="s">
         <v>4472</v>
       </c>
-      <c r="F1972" s="53"/>
+      <c r="F1972" s="81"/>
       <c r="G1972" s="53"/>
       <c r="H1972" s="53"/>
       <c r="I1972" s="53"/>
@@ -28969,7 +29318,7 @@
       <c r="C1973" s="62"/>
       <c r="D1973" s="55"/>
       <c r="E1973" s="3"/>
-      <c r="F1973" s="53"/>
+      <c r="F1973" s="81"/>
       <c r="G1973" s="53"/>
       <c r="H1973" s="53"/>
       <c r="I1973" s="53"/>
@@ -28992,7 +29341,7 @@
       <c r="C1974" s="62"/>
       <c r="D1974" s="55"/>
       <c r="E1974" s="3"/>
-      <c r="F1974" s="53"/>
+      <c r="F1974" s="81"/>
       <c r="G1974" s="53"/>
       <c r="H1974" s="53"/>
       <c r="I1974" s="53"/>
@@ -29015,7 +29364,7 @@
       <c r="C1975" s="62"/>
       <c r="D1975" s="55"/>
       <c r="E1975" s="3"/>
-      <c r="F1975" s="53"/>
+      <c r="F1975" s="81"/>
       <c r="G1975" s="53"/>
       <c r="H1975" s="53"/>
       <c r="I1975" s="53"/>
@@ -29038,7 +29387,7 @@
       <c r="C1976" s="62"/>
       <c r="D1976" s="55"/>
       <c r="E1976" s="3"/>
-      <c r="F1976" s="53"/>
+      <c r="F1976" s="81"/>
       <c r="G1976" s="53"/>
       <c r="H1976" s="53"/>
       <c r="I1976" s="53"/>
@@ -29061,7 +29410,7 @@
       <c r="C1977" s="62"/>
       <c r="D1977" s="55"/>
       <c r="E1977" s="53"/>
-      <c r="F1977" s="53" t="s">
+      <c r="F1977" s="81" t="s">
         <v>4460</v>
       </c>
       <c r="G1977" s="53"/>
@@ -29088,7 +29437,9 @@
       <c r="E1978" s="3" t="s">
         <v>4473</v>
       </c>
-      <c r="F1978" s="53"/>
+      <c r="F1978" s="81" t="s">
+        <v>4505</v>
+      </c>
       <c r="G1978" s="53"/>
       <c r="H1978" s="53"/>
       <c r="I1978" s="53"/>
@@ -29111,7 +29462,7 @@
       <c r="C1979" s="62"/>
       <c r="D1979" s="55"/>
       <c r="E1979" s="3"/>
-      <c r="F1979" s="53"/>
+      <c r="F1979" s="81"/>
       <c r="G1979" s="53"/>
       <c r="H1979" s="53"/>
       <c r="I1979" s="53"/>
@@ -29134,7 +29485,7 @@
       <c r="C1980" s="62"/>
       <c r="D1980" s="55"/>
       <c r="E1980" s="3"/>
-      <c r="F1980" s="53"/>
+      <c r="F1980" s="81"/>
       <c r="G1980" s="53"/>
       <c r="H1980" s="53"/>
       <c r="I1980" s="53"/>
@@ -29157,7 +29508,7 @@
       <c r="C1981" s="62"/>
       <c r="D1981" s="55"/>
       <c r="E1981" s="3"/>
-      <c r="F1981" s="53"/>
+      <c r="F1981" s="81"/>
       <c r="G1981" s="53"/>
       <c r="H1981" s="53"/>
       <c r="I1981" s="53"/>
@@ -29182,7 +29533,7 @@
       <c r="E1982" s="3" t="s">
         <v>4475</v>
       </c>
-      <c r="F1982" s="53"/>
+      <c r="F1982" s="81"/>
       <c r="G1982" s="53"/>
       <c r="H1982" s="53"/>
       <c r="I1982" s="53"/>
@@ -29205,7 +29556,9 @@
       <c r="C1983" s="62"/>
       <c r="D1983" s="55"/>
       <c r="E1983" s="3"/>
-      <c r="F1983" s="53"/>
+      <c r="F1983" s="81" t="s">
+        <v>4507</v>
+      </c>
       <c r="G1983" s="53"/>
       <c r="H1983" s="53"/>
       <c r="I1983" s="53"/>
@@ -29228,22 +29581,30 @@
       <c r="C1984" s="62"/>
       <c r="D1984" s="55"/>
       <c r="E1984" s="3"/>
-      <c r="F1984" s="53"/>
-      <c r="G1984" s="53"/>
-      <c r="H1984" s="53"/>
-      <c r="I1984" s="53"/>
+      <c r="F1984" s="81"/>
+      <c r="G1984" s="53" t="s">
+        <v>4508</v>
+      </c>
+      <c r="H1984" s="53" t="s">
+        <v>4303</v>
+      </c>
+      <c r="I1984" s="53" t="s">
+        <v>4519</v>
+      </c>
       <c r="J1984" s="53"/>
       <c r="K1984" s="53"/>
       <c r="L1984" s="53"/>
       <c r="M1984" s="53"/>
-      <c r="N1984" s="53"/>
+      <c r="N1984" s="53" t="s">
+        <v>4520</v>
+      </c>
       <c r="O1984" s="53"/>
       <c r="P1984" s="53"/>
       <c r="Q1984" s="66"/>
       <c r="R1984" s="42"/>
       <c r="S1984" s="42"/>
     </row>
-    <row r="1985" spans="1:19">
+    <row r="1985" spans="1:19" ht="40.500000">
       <c r="A1985" s="58" t="s">
         <v>125</v>
       </c>
@@ -29251,10 +29612,14 @@
       <c r="C1985" s="62"/>
       <c r="D1985" s="55"/>
       <c r="E1985" s="3"/>
-      <c r="F1985" s="53"/>
+      <c r="F1985" s="81" t="s">
+        <v>4517</v>
+      </c>
       <c r="G1985" s="53"/>
       <c r="H1985" s="53"/>
-      <c r="I1985" s="53"/>
+      <c r="I1985" s="53" t="s">
+        <v>4518</v>
+      </c>
       <c r="J1985" s="53"/>
       <c r="K1985" s="53"/>
       <c r="L1985" s="53"/>
@@ -29266,28 +29631,30 @@
       <c r="R1985" s="42"/>
       <c r="S1985" s="42"/>
     </row>
-    <row r="1986" spans="1:19">
+    <row r="1986" spans="1:19" ht="40.500000">
       <c r="A1986" s="58" t="s">
         <v>126</v>
       </c>
       <c r="B1986" s="61"/>
       <c r="C1986" s="62"/>
       <c r="D1986" s="55"/>
-      <c r="E1986" s="3" t="s">
+      <c r="E1986" s="85" t="s">
         <v>4476</v>
       </c>
-      <c r="F1986" s="53"/>
-      <c r="G1986" s="53"/>
-      <c r="H1986" s="53"/>
-      <c r="I1986" s="53"/>
-      <c r="J1986" s="53"/>
-      <c r="K1986" s="53"/>
-      <c r="L1986" s="53"/>
-      <c r="M1986" s="53"/>
-      <c r="N1986" s="53"/>
-      <c r="O1986" s="53"/>
-      <c r="P1986" s="53"/>
-      <c r="Q1986" s="66"/>
+      <c r="F1986" s="86"/>
+      <c r="G1986" s="87"/>
+      <c r="H1986" s="87"/>
+      <c r="I1986" s="87"/>
+      <c r="J1986" s="87"/>
+      <c r="K1986" s="87"/>
+      <c r="L1986" s="87" t="s">
+        <v>4523</v>
+      </c>
+      <c r="M1986" s="87"/>
+      <c r="N1986" s="87"/>
+      <c r="O1986" s="87"/>
+      <c r="P1986" s="87"/>
+      <c r="Q1986" s="88"/>
       <c r="R1986" s="42"/>
       <c r="S1986" s="42"/>
     </row>
@@ -29299,7 +29666,7 @@
       <c r="C1987" s="62"/>
       <c r="D1987" s="55"/>
       <c r="E1987" s="3"/>
-      <c r="F1987" s="53"/>
+      <c r="F1987" s="81"/>
       <c r="G1987" s="53"/>
       <c r="H1987" s="53"/>
       <c r="I1987" s="53"/>
@@ -29307,7 +29674,9 @@
       <c r="K1987" s="53"/>
       <c r="L1987" s="53"/>
       <c r="M1987" s="53"/>
-      <c r="N1987" s="53"/>
+      <c r="N1987" s="53" t="s">
+        <v>4524</v>
+      </c>
       <c r="O1987" s="53"/>
       <c r="P1987" s="53"/>
       <c r="Q1987" s="66"/>
@@ -29322,15 +29691,19 @@
       <c r="C1988" s="62"/>
       <c r="D1988" s="55"/>
       <c r="E1988" s="3"/>
-      <c r="F1988" s="53"/>
-      <c r="G1988" s="53"/>
+      <c r="F1988" s="81"/>
+      <c r="G1988" s="53" t="s">
+        <v>4525</v>
+      </c>
       <c r="H1988" s="53"/>
       <c r="I1988" s="53"/>
       <c r="J1988" s="53"/>
       <c r="K1988" s="53"/>
       <c r="L1988" s="53"/>
       <c r="M1988" s="53"/>
-      <c r="N1988" s="53"/>
+      <c r="N1988" s="53" t="s">
+        <v>4526</v>
+      </c>
       <c r="O1988" s="53"/>
       <c r="P1988" s="53"/>
       <c r="Q1988" s="66"/>
@@ -29344,19 +29717,23 @@
       <c r="B1989" s="61"/>
       <c r="C1989" s="62"/>
       <c r="D1989" s="55"/>
-      <c r="E1989" s="3"/>
-      <c r="F1989" s="53"/>
-      <c r="G1989" s="53"/>
-      <c r="H1989" s="53"/>
-      <c r="I1989" s="53"/>
-      <c r="J1989" s="53"/>
-      <c r="K1989" s="53"/>
-      <c r="L1989" s="53"/>
-      <c r="M1989" s="53"/>
-      <c r="N1989" s="53"/>
-      <c r="O1989" s="53"/>
-      <c r="P1989" s="53"/>
-      <c r="Q1989" s="66"/>
+      <c r="E1989" s="89"/>
+      <c r="F1989" s="90"/>
+      <c r="G1989" s="91"/>
+      <c r="H1989" s="91" t="s">
+        <v>4527</v>
+      </c>
+      <c r="I1989" s="91"/>
+      <c r="J1989" s="91"/>
+      <c r="K1989" s="91"/>
+      <c r="L1989" s="91"/>
+      <c r="M1989" s="91"/>
+      <c r="N1989" s="91"/>
+      <c r="O1989" s="91" t="s">
+        <v>4528</v>
+      </c>
+      <c r="P1989" s="91"/>
+      <c r="Q1989" s="92"/>
       <c r="R1989" s="42"/>
       <c r="S1989" s="42"/>
     </row>
@@ -29367,23 +29744,23 @@
       <c r="B1990" s="61"/>
       <c r="C1990" s="62"/>
       <c r="D1990" s="55"/>
-      <c r="E1990" s="3" t="s">
+      <c r="E1990" s="85" t="s">
         <v>4461</v>
       </c>
-      <c r="F1990" s="53"/>
-      <c r="G1990" s="53"/>
-      <c r="H1990" s="53"/>
-      <c r="I1990" s="53"/>
-      <c r="J1990" s="53"/>
-      <c r="K1990" s="53"/>
-      <c r="L1990" s="53"/>
-      <c r="M1990" s="53"/>
-      <c r="N1990" s="53"/>
-      <c r="O1990" s="53"/>
-      <c r="P1990" s="53" t="s">
+      <c r="F1990" s="86"/>
+      <c r="G1990" s="87"/>
+      <c r="H1990" s="87"/>
+      <c r="I1990" s="87"/>
+      <c r="J1990" s="87"/>
+      <c r="K1990" s="87"/>
+      <c r="L1990" s="87"/>
+      <c r="M1990" s="87"/>
+      <c r="N1990" s="87"/>
+      <c r="O1990" s="87"/>
+      <c r="P1990" s="87" t="s">
         <v>4462</v>
       </c>
-      <c r="Q1990" s="66"/>
+      <c r="Q1990" s="88"/>
       <c r="R1990" s="42"/>
       <c r="S1990" s="42"/>
     </row>
@@ -29395,10 +29772,16 @@
       <c r="C1991" s="62"/>
       <c r="D1991" s="55"/>
       <c r="E1991" s="3"/>
-      <c r="F1991" s="53"/>
+      <c r="F1991" s="81" t="s">
+        <v>4510</v>
+      </c>
       <c r="G1991" s="53"/>
-      <c r="H1991" s="53"/>
-      <c r="I1991" s="53"/>
+      <c r="H1991" s="53" t="s">
+        <v>4515</v>
+      </c>
+      <c r="I1991" s="53" t="s">
+        <v>4529</v>
+      </c>
       <c r="J1991" s="53"/>
       <c r="K1991" s="53"/>
       <c r="L1991" s="53" t="s">
@@ -29407,14 +29790,16 @@
       <c r="M1991" s="53" t="s">
         <v>4464</v>
       </c>
-      <c r="N1991" s="53"/>
+      <c r="N1991" s="53" t="s">
+        <v>4530</v>
+      </c>
       <c r="O1991" s="53"/>
       <c r="P1991" s="53"/>
       <c r="Q1991" s="66"/>
       <c r="R1991" s="42"/>
       <c r="S1991" s="42"/>
     </row>
-    <row r="1992" spans="1:19">
+    <row r="1992" spans="1:19" ht="54.000000">
       <c r="A1992" s="58" t="s">
         <v>132</v>
       </c>
@@ -29422,45 +29807,59 @@
       <c r="C1992" s="62"/>
       <c r="D1992" s="55"/>
       <c r="E1992" s="3"/>
-      <c r="F1992" s="53"/>
+      <c r="F1992" s="81" t="s">
+        <v>4531</v>
+      </c>
       <c r="G1992" s="53"/>
-      <c r="H1992" s="53"/>
+      <c r="H1992" s="53" t="s">
+        <v>4532</v>
+      </c>
       <c r="I1992" s="53"/>
-      <c r="J1992" s="53"/>
-      <c r="K1992" s="53"/>
+      <c r="J1992" s="53" t="s">
+        <v>4534</v>
+      </c>
+      <c r="K1992" s="53" t="s">
+        <v>4536</v>
+      </c>
       <c r="L1992" s="53"/>
       <c r="M1992" s="53"/>
-      <c r="N1992" s="53"/>
+      <c r="N1992" s="53" t="s">
+        <v>4537</v>
+      </c>
       <c r="O1992" s="53"/>
       <c r="P1992" s="53"/>
       <c r="Q1992" s="66"/>
       <c r="R1992" s="42"/>
       <c r="S1992" s="42"/>
     </row>
-    <row r="1993" spans="1:19">
+    <row r="1993" spans="1:19" ht="40.500000">
       <c r="A1993" s="58" t="s">
         <v>133</v>
       </c>
       <c r="B1993" s="61"/>
       <c r="C1993" s="62"/>
       <c r="D1993" s="55"/>
-      <c r="E1993" s="3"/>
-      <c r="F1993" s="53"/>
-      <c r="G1993" s="53"/>
-      <c r="H1993" s="53"/>
-      <c r="I1993" s="53"/>
-      <c r="J1993" s="53"/>
-      <c r="K1993" s="53"/>
-      <c r="L1993" s="53"/>
-      <c r="M1993" s="53"/>
-      <c r="N1993" s="53"/>
-      <c r="O1993" s="53"/>
-      <c r="P1993" s="53"/>
-      <c r="Q1993" s="66"/>
+      <c r="E1993" s="89"/>
+      <c r="F1993" s="90" t="s">
+        <v>4538</v>
+      </c>
+      <c r="G1993" s="91"/>
+      <c r="H1993" s="91"/>
+      <c r="I1993" s="91"/>
+      <c r="J1993" s="91"/>
+      <c r="K1993" s="91"/>
+      <c r="L1993" s="91"/>
+      <c r="M1993" s="91"/>
+      <c r="N1993" s="91" t="s">
+        <v>4539</v>
+      </c>
+      <c r="O1993" s="91"/>
+      <c r="P1993" s="91"/>
+      <c r="Q1993" s="92"/>
       <c r="R1993" s="42"/>
       <c r="S1993" s="42"/>
     </row>
-    <row r="1994" spans="1:19">
+    <row r="1994" spans="1:19" ht="54.000000">
       <c r="A1994" s="58" t="s">
         <v>134</v>
       </c>
@@ -29470,13 +29869,17 @@
       <c r="E1994" s="3" t="s">
         <v>4465</v>
       </c>
-      <c r="F1994" s="53"/>
-      <c r="G1994" s="53"/>
+      <c r="F1994" s="81"/>
+      <c r="G1994" s="53" t="s">
+        <v>4534</v>
+      </c>
       <c r="H1994" s="53"/>
       <c r="I1994" s="53"/>
       <c r="J1994" s="53"/>
       <c r="K1994" s="53"/>
-      <c r="L1994" s="53"/>
+      <c r="L1994" s="53" t="s">
+        <v>4542</v>
+      </c>
       <c r="M1994" s="53"/>
       <c r="N1994" s="53"/>
       <c r="O1994" s="53"/>
@@ -29485,7 +29888,7 @@
       <c r="R1994" s="42"/>
       <c r="S1994" s="42"/>
     </row>
-    <row r="1995" spans="1:19">
+    <row r="1995" spans="1:19" ht="40.500000">
       <c r="A1995" s="58" t="s">
         <v>135</v>
       </c>
@@ -29493,7 +29896,9 @@
       <c r="C1995" s="62"/>
       <c r="D1995" s="55"/>
       <c r="E1995" s="3"/>
-      <c r="F1995" s="53"/>
+      <c r="F1995" s="81" t="s">
+        <v>4543</v>
+      </c>
       <c r="G1995" s="53" t="s">
         <v>4467</v>
       </c>
@@ -29512,7 +29917,7 @@
       <c r="R1995" s="42"/>
       <c r="S1995" s="42"/>
     </row>
-    <row r="1996" spans="1:19">
+    <row r="1996" spans="1:19" ht="54.000000">
       <c r="A1996" s="58" t="s">
         <v>4241</v>
       </c>
@@ -29522,18 +29927,22 @@
         <v>4399</v>
       </c>
       <c r="E1996" s="53"/>
-      <c r="F1996" s="75" t="s">
+      <c r="F1996" s="84" t="s">
         <v>4290</v>
       </c>
       <c r="G1996" s="53"/>
       <c r="H1996" s="53"/>
       <c r="I1996" s="53"/>
       <c r="J1996" s="53"/>
-      <c r="K1996" s="53"/>
+      <c r="K1996" s="53" t="s">
+        <v>4544</v>
+      </c>
       <c r="L1996" s="53"/>
       <c r="M1996" s="53"/>
       <c r="N1996" s="53"/>
-      <c r="O1996" s="53"/>
+      <c r="O1996" s="53" t="s">
+        <v>4545</v>
+      </c>
       <c r="P1996" s="53"/>
       <c r="Q1996" s="66"/>
     </row>
@@ -29545,7 +29954,7 @@
       <c r="C1997" s="62"/>
       <c r="D1997" s="3"/>
       <c r="E1997" s="53"/>
-      <c r="F1997" s="53"/>
+      <c r="F1997" s="81"/>
       <c r="G1997" s="53"/>
       <c r="H1997" s="53"/>
       <c r="I1997" s="53"/>
@@ -29568,7 +29977,7 @@
       <c r="C1998" s="62"/>
       <c r="D1998" s="3"/>
       <c r="E1998" s="53"/>
-      <c r="F1998" s="53"/>
+      <c r="F1998" s="81"/>
       <c r="G1998" s="53"/>
       <c r="H1998" s="53"/>
       <c r="I1998" s="53"/>
@@ -29591,7 +30000,7 @@
       <c r="C1999" s="62"/>
       <c r="D1999" s="3"/>
       <c r="E1999" s="53"/>
-      <c r="F1999" s="53"/>
+      <c r="F1999" s="81"/>
       <c r="G1999" s="53"/>
       <c r="H1999" s="53"/>
       <c r="I1999" s="53"/>
@@ -29614,7 +30023,7 @@
       <c r="C2000" s="62"/>
       <c r="D2000" s="3"/>
       <c r="E2000" s="53"/>
-      <c r="F2000" s="53"/>
+      <c r="F2000" s="81"/>
       <c r="G2000" s="53"/>
       <c r="H2000" s="53"/>
       <c r="I2000" s="53"/>
@@ -29637,7 +30046,7 @@
       <c r="C2001" s="62"/>
       <c r="D2001" s="3"/>
       <c r="E2001" s="53"/>
-      <c r="F2001" s="53"/>
+      <c r="F2001" s="81"/>
       <c r="G2001" s="53"/>
       <c r="H2001" s="53"/>
       <c r="I2001" s="53"/>
@@ -29660,7 +30069,7 @@
       <c r="C2002" s="62"/>
       <c r="D2002" s="3"/>
       <c r="E2002" s="53"/>
-      <c r="F2002" s="53"/>
+      <c r="F2002" s="81"/>
       <c r="G2002" s="53"/>
       <c r="H2002" s="53"/>
       <c r="I2002" s="53"/>
@@ -29683,7 +30092,7 @@
       <c r="C2003" s="62"/>
       <c r="D2003" s="3"/>
       <c r="E2003" s="53"/>
-      <c r="F2003" s="53"/>
+      <c r="F2003" s="81"/>
       <c r="G2003" s="53"/>
       <c r="H2003" s="53"/>
       <c r="I2003" s="53"/>
@@ -29706,7 +30115,7 @@
       <c r="C2004" s="62"/>
       <c r="D2004" s="3"/>
       <c r="E2004" s="53"/>
-      <c r="F2004" s="53"/>
+      <c r="F2004" s="81"/>
       <c r="G2004" s="53"/>
       <c r="H2004" s="53"/>
       <c r="I2004" s="53"/>
@@ -29729,7 +30138,7 @@
       <c r="C2005" s="62"/>
       <c r="D2005" s="3"/>
       <c r="E2005" s="53"/>
-      <c r="F2005" s="53"/>
+      <c r="F2005" s="81"/>
       <c r="G2005" s="53"/>
       <c r="H2005" s="53"/>
       <c r="I2005" s="53"/>
@@ -29752,7 +30161,7 @@
       <c r="C2006" s="62"/>
       <c r="D2006" s="3"/>
       <c r="E2006" s="53"/>
-      <c r="F2006" s="53"/>
+      <c r="F2006" s="81"/>
       <c r="G2006" s="53"/>
       <c r="H2006" s="53"/>
       <c r="I2006" s="53"/>
@@ -29775,7 +30184,7 @@
       <c r="C2007" s="62"/>
       <c r="D2007" s="3"/>
       <c r="E2007" s="53"/>
-      <c r="F2007" s="53"/>
+      <c r="F2007" s="81"/>
       <c r="G2007" s="53"/>
       <c r="H2007" s="53"/>
       <c r="I2007" s="53"/>
@@ -29798,7 +30207,7 @@
       <c r="C2008" s="62"/>
       <c r="D2008" s="3"/>
       <c r="E2008" s="53"/>
-      <c r="F2008" s="53"/>
+      <c r="F2008" s="81"/>
       <c r="G2008" s="53"/>
       <c r="H2008" s="53"/>
       <c r="I2008" s="53"/>
@@ -29821,7 +30230,7 @@
       <c r="C2009" s="62"/>
       <c r="D2009" s="3"/>
       <c r="E2009" s="53"/>
-      <c r="F2009" s="53"/>
+      <c r="F2009" s="81"/>
       <c r="G2009" s="53"/>
       <c r="H2009" s="53"/>
       <c r="I2009" s="53"/>
@@ -29846,7 +30255,7 @@
         <v>4372</v>
       </c>
       <c r="E2010" s="53"/>
-      <c r="F2010" s="53"/>
+      <c r="F2010" s="81"/>
       <c r="G2010" s="53"/>
       <c r="H2010" s="53"/>
       <c r="I2010" s="53"/>
@@ -29867,7 +30276,7 @@
       <c r="C2011" s="62"/>
       <c r="D2011" s="3"/>
       <c r="E2011" s="53"/>
-      <c r="F2011" s="53"/>
+      <c r="F2011" s="81"/>
       <c r="G2011" s="53"/>
       <c r="H2011" s="53"/>
       <c r="I2011" s="53"/>
@@ -29890,7 +30299,7 @@
       <c r="C2012" s="62"/>
       <c r="D2012" s="3"/>
       <c r="E2012" s="53"/>
-      <c r="F2012" s="53"/>
+      <c r="F2012" s="81"/>
       <c r="G2012" s="53"/>
       <c r="H2012" s="53"/>
       <c r="I2012" s="53"/>
@@ -29913,7 +30322,7 @@
       <c r="C2013" s="62"/>
       <c r="D2013" s="3"/>
       <c r="E2013" s="53"/>
-      <c r="F2013" s="53"/>
+      <c r="F2013" s="81"/>
       <c r="G2013" s="53"/>
       <c r="H2013" s="53"/>
       <c r="I2013" s="53"/>
@@ -29936,7 +30345,7 @@
       <c r="C2014" s="62"/>
       <c r="D2014" s="3"/>
       <c r="E2014" s="53"/>
-      <c r="F2014" s="53"/>
+      <c r="F2014" s="81"/>
       <c r="G2014" s="53"/>
       <c r="H2014" s="53"/>
       <c r="I2014" s="53"/>
@@ -29959,7 +30368,7 @@
       <c r="C2015" s="62"/>
       <c r="D2015" s="3"/>
       <c r="E2015" s="53"/>
-      <c r="F2015" s="53"/>
+      <c r="F2015" s="81"/>
       <c r="G2015" s="53"/>
       <c r="H2015" s="53"/>
       <c r="I2015" s="53"/>
@@ -29982,7 +30391,7 @@
       <c r="C2016" s="62"/>
       <c r="D2016" s="3"/>
       <c r="E2016" s="53"/>
-      <c r="F2016" s="53"/>
+      <c r="F2016" s="81"/>
       <c r="G2016" s="53"/>
       <c r="H2016" s="53"/>
       <c r="I2016" s="53"/>
@@ -30005,7 +30414,7 @@
       <c r="C2017" s="62"/>
       <c r="D2017" s="3"/>
       <c r="E2017" s="53"/>
-      <c r="F2017" s="53"/>
+      <c r="F2017" s="81"/>
       <c r="G2017" s="53"/>
       <c r="H2017" s="53"/>
       <c r="I2017" s="53"/>
@@ -30028,7 +30437,7 @@
       <c r="C2018" s="62"/>
       <c r="D2018" s="3"/>
       <c r="E2018" s="53"/>
-      <c r="F2018" s="53"/>
+      <c r="F2018" s="81"/>
       <c r="G2018" s="53"/>
       <c r="H2018" s="53"/>
       <c r="I2018" s="53"/>
@@ -30051,7 +30460,7 @@
       <c r="C2019" s="62"/>
       <c r="D2019" s="3"/>
       <c r="E2019" s="53"/>
-      <c r="F2019" s="53"/>
+      <c r="F2019" s="81"/>
       <c r="G2019" s="53"/>
       <c r="H2019" s="53"/>
       <c r="I2019" s="53"/>
@@ -30074,7 +30483,7 @@
       <c r="C2020" s="62"/>
       <c r="D2020" s="3"/>
       <c r="E2020" s="53"/>
-      <c r="F2020" s="53"/>
+      <c r="F2020" s="81"/>
       <c r="G2020" s="53"/>
       <c r="H2020" s="53"/>
       <c r="I2020" s="53"/>
@@ -30097,7 +30506,7 @@
       <c r="C2021" s="62"/>
       <c r="D2021" s="3"/>
       <c r="E2021" s="53"/>
-      <c r="F2021" s="53"/>
+      <c r="F2021" s="81"/>
       <c r="G2021" s="53"/>
       <c r="H2021" s="53"/>
       <c r="I2021" s="53"/>
@@ -30120,7 +30529,7 @@
       <c r="C2022" s="62"/>
       <c r="D2022" s="3"/>
       <c r="E2022" s="53"/>
-      <c r="F2022" s="53"/>
+      <c r="F2022" s="81"/>
       <c r="G2022" s="53"/>
       <c r="H2022" s="53"/>
       <c r="I2022" s="53"/>
@@ -30143,7 +30552,7 @@
       <c r="C2023" s="62"/>
       <c r="D2023" s="3"/>
       <c r="E2023" s="53"/>
-      <c r="F2023" s="53"/>
+      <c r="F2023" s="81"/>
       <c r="G2023" s="53"/>
       <c r="H2023" s="53"/>
       <c r="I2023" s="53"/>
@@ -30166,7 +30575,7 @@
       <c r="C2024" s="62"/>
       <c r="D2024" s="3"/>
       <c r="E2024" s="53"/>
-      <c r="F2024" s="53"/>
+      <c r="F2024" s="81"/>
       <c r="G2024" s="53"/>
       <c r="H2024" s="53"/>
       <c r="I2024" s="53"/>
@@ -30189,7 +30598,7 @@
       <c r="C2025" s="62"/>
       <c r="D2025" s="3"/>
       <c r="E2025" s="53"/>
-      <c r="F2025" s="53"/>
+      <c r="F2025" s="81"/>
       <c r="G2025" s="53"/>
       <c r="H2025" s="53"/>
       <c r="I2025" s="53"/>
@@ -30212,7 +30621,7 @@
       <c r="C2026" s="62"/>
       <c r="D2026" s="3"/>
       <c r="E2026" s="53"/>
-      <c r="F2026" s="53"/>
+      <c r="F2026" s="81"/>
       <c r="G2026" s="53"/>
       <c r="H2026" s="53"/>
       <c r="I2026" s="53"/>
@@ -30235,7 +30644,7 @@
       <c r="C2027" s="62"/>
       <c r="D2027" s="3"/>
       <c r="E2027" s="53"/>
-      <c r="F2027" s="53"/>
+      <c r="F2027" s="81"/>
       <c r="G2027" s="53"/>
       <c r="H2027" s="53"/>
       <c r="I2027" s="53"/>
@@ -30258,7 +30667,7 @@
       <c r="C2028" s="62"/>
       <c r="D2028" s="3"/>
       <c r="E2028" s="53"/>
-      <c r="F2028" s="53"/>
+      <c r="F2028" s="81"/>
       <c r="G2028" s="53"/>
       <c r="H2028" s="53"/>
       <c r="I2028" s="53"/>
@@ -30281,7 +30690,7 @@
       <c r="C2029" s="62"/>
       <c r="D2029" s="3"/>
       <c r="E2029" s="53"/>
-      <c r="F2029" s="53"/>
+      <c r="F2029" s="81"/>
       <c r="G2029" s="53"/>
       <c r="H2029" s="53"/>
       <c r="I2029" s="53"/>
@@ -30304,7 +30713,7 @@
       <c r="C2030" s="62"/>
       <c r="D2030" s="3"/>
       <c r="E2030" s="53"/>
-      <c r="F2030" s="53"/>
+      <c r="F2030" s="81"/>
       <c r="G2030" s="53"/>
       <c r="H2030" s="53"/>
       <c r="I2030" s="53"/>
@@ -30327,7 +30736,7 @@
       <c r="C2031" s="62"/>
       <c r="D2031" s="3"/>
       <c r="E2031" s="53"/>
-      <c r="F2031" s="53"/>
+      <c r="F2031" s="81"/>
       <c r="G2031" s="53"/>
       <c r="H2031" s="53"/>
       <c r="I2031" s="53"/>
@@ -30350,7 +30759,7 @@
       <c r="C2032" s="62"/>
       <c r="D2032" s="3"/>
       <c r="E2032" s="53"/>
-      <c r="F2032" s="53"/>
+      <c r="F2032" s="81"/>
       <c r="G2032" s="53"/>
       <c r="H2032" s="53"/>
       <c r="I2032" s="53"/>
@@ -30373,7 +30782,7 @@
       <c r="C2033" s="62"/>
       <c r="D2033" s="3"/>
       <c r="E2033" s="53"/>
-      <c r="F2033" s="53"/>
+      <c r="F2033" s="81"/>
       <c r="G2033" s="53"/>
       <c r="H2033" s="53"/>
       <c r="I2033" s="53"/>
@@ -30396,7 +30805,7 @@
       <c r="C2034" s="62"/>
       <c r="D2034" s="3"/>
       <c r="E2034" s="53"/>
-      <c r="F2034" s="53"/>
+      <c r="F2034" s="81"/>
       <c r="G2034" s="53"/>
       <c r="H2034" s="53"/>
       <c r="I2034" s="53"/>
@@ -30419,7 +30828,7 @@
       <c r="C2035" s="62"/>
       <c r="D2035" s="3"/>
       <c r="E2035" s="53"/>
-      <c r="F2035" s="53"/>
+      <c r="F2035" s="81"/>
       <c r="G2035" s="53"/>
       <c r="H2035" s="53"/>
       <c r="I2035" s="53"/>
@@ -30444,7 +30853,7 @@
         <v>4400</v>
       </c>
       <c r="E2036" s="53"/>
-      <c r="F2036" s="53"/>
+      <c r="F2036" s="81"/>
       <c r="G2036" s="53"/>
       <c r="H2036" s="53"/>
       <c r="I2036" s="53"/>
@@ -30465,7 +30874,7 @@
       <c r="C2037" s="62"/>
       <c r="D2037" s="3"/>
       <c r="E2037" s="53"/>
-      <c r="F2037" s="53"/>
+      <c r="F2037" s="81"/>
       <c r="G2037" s="53"/>
       <c r="H2037" s="53"/>
       <c r="I2037" s="53"/>
@@ -30488,7 +30897,7 @@
       <c r="C2038" s="62"/>
       <c r="D2038" s="3"/>
       <c r="E2038" s="53"/>
-      <c r="F2038" s="53"/>
+      <c r="F2038" s="81"/>
       <c r="G2038" s="53"/>
       <c r="H2038" s="53"/>
       <c r="I2038" s="53"/>
@@ -30511,7 +30920,7 @@
       <c r="C2039" s="62"/>
       <c r="D2039" s="3"/>
       <c r="E2039" s="53"/>
-      <c r="F2039" s="53"/>
+      <c r="F2039" s="81"/>
       <c r="G2039" s="53"/>
       <c r="H2039" s="53"/>
       <c r="I2039" s="53"/>
@@ -30534,7 +30943,7 @@
       <c r="C2040" s="62"/>
       <c r="D2040" s="3"/>
       <c r="E2040" s="53"/>
-      <c r="F2040" s="53"/>
+      <c r="F2040" s="81"/>
       <c r="G2040" s="53"/>
       <c r="H2040" s="53"/>
       <c r="I2040" s="53"/>
@@ -30557,7 +30966,7 @@
       <c r="C2041" s="62"/>
       <c r="D2041" s="3"/>
       <c r="E2041" s="53"/>
-      <c r="F2041" s="53"/>
+      <c r="F2041" s="81"/>
       <c r="G2041" s="53"/>
       <c r="H2041" s="53"/>
       <c r="I2041" s="53"/>
@@ -30580,7 +30989,7 @@
       <c r="C2042" s="62"/>
       <c r="D2042" s="3"/>
       <c r="E2042" s="53"/>
-      <c r="F2042" s="53"/>
+      <c r="F2042" s="81"/>
       <c r="G2042" s="53"/>
       <c r="H2042" s="53"/>
       <c r="I2042" s="53"/>
@@ -30603,7 +31012,7 @@
       <c r="C2043" s="62"/>
       <c r="D2043" s="3"/>
       <c r="E2043" s="53"/>
-      <c r="F2043" s="53"/>
+      <c r="F2043" s="81"/>
       <c r="G2043" s="53"/>
       <c r="H2043" s="53"/>
       <c r="I2043" s="53"/>
@@ -30626,7 +31035,7 @@
       <c r="C2044" s="62"/>
       <c r="D2044" s="3"/>
       <c r="E2044" s="53"/>
-      <c r="F2044" s="53"/>
+      <c r="F2044" s="81"/>
       <c r="G2044" s="53"/>
       <c r="H2044" s="53"/>
       <c r="I2044" s="53"/>
@@ -30649,7 +31058,7 @@
       <c r="C2045" s="62"/>
       <c r="D2045" s="3"/>
       <c r="E2045" s="53"/>
-      <c r="F2045" s="53"/>
+      <c r="F2045" s="81"/>
       <c r="G2045" s="53"/>
       <c r="H2045" s="53"/>
       <c r="I2045" s="53"/>
@@ -30672,7 +31081,7 @@
       <c r="C2046" s="62"/>
       <c r="D2046" s="3"/>
       <c r="E2046" s="53"/>
-      <c r="F2046" s="53"/>
+      <c r="F2046" s="81"/>
       <c r="G2046" s="53"/>
       <c r="H2046" s="53"/>
       <c r="I2046" s="53"/>
@@ -30695,7 +31104,7 @@
       <c r="C2047" s="62"/>
       <c r="D2047" s="3"/>
       <c r="E2047" s="53"/>
-      <c r="F2047" s="53"/>
+      <c r="F2047" s="81"/>
       <c r="G2047" s="53"/>
       <c r="H2047" s="53"/>
       <c r="I2047" s="53"/>
@@ -30718,7 +31127,7 @@
       <c r="C2048" s="62"/>
       <c r="D2048" s="3"/>
       <c r="E2048" s="53"/>
-      <c r="F2048" s="53"/>
+      <c r="F2048" s="81"/>
       <c r="G2048" s="53"/>
       <c r="H2048" s="53"/>
       <c r="I2048" s="53"/>
@@ -30741,7 +31150,7 @@
       <c r="C2049" s="62"/>
       <c r="D2049" s="3"/>
       <c r="E2049" s="53"/>
-      <c r="F2049" s="53"/>
+      <c r="F2049" s="81"/>
       <c r="G2049" s="53"/>
       <c r="H2049" s="53"/>
       <c r="I2049" s="53"/>
@@ -30764,7 +31173,7 @@
       <c r="C2050" s="62"/>
       <c r="D2050" s="3"/>
       <c r="E2050" s="53"/>
-      <c r="F2050" s="53"/>
+      <c r="F2050" s="81"/>
       <c r="G2050" s="53"/>
       <c r="H2050" s="53"/>
       <c r="I2050" s="53"/>
@@ -30787,7 +31196,7 @@
       <c r="C2051" s="62"/>
       <c r="D2051" s="3"/>
       <c r="E2051" s="53"/>
-      <c r="F2051" s="53"/>
+      <c r="F2051" s="81"/>
       <c r="G2051" s="53"/>
       <c r="H2051" s="53"/>
       <c r="I2051" s="53"/>
@@ -30810,7 +31219,7 @@
       <c r="C2052" s="62"/>
       <c r="D2052" s="3"/>
       <c r="E2052" s="53"/>
-      <c r="F2052" s="53"/>
+      <c r="F2052" s="81"/>
       <c r="G2052" s="53"/>
       <c r="H2052" s="53"/>
       <c r="I2052" s="53"/>
@@ -30835,7 +31244,7 @@
         <v>4401</v>
       </c>
       <c r="E2053" s="53"/>
-      <c r="F2053" s="53"/>
+      <c r="F2053" s="81"/>
       <c r="G2053" s="53"/>
       <c r="H2053" s="53"/>
       <c r="I2053" s="53"/>
@@ -30856,7 +31265,7 @@
       <c r="C2054" s="62"/>
       <c r="D2054" s="3"/>
       <c r="E2054" s="53"/>
-      <c r="F2054" s="53"/>
+      <c r="F2054" s="81"/>
       <c r="G2054" s="53"/>
       <c r="H2054" s="53"/>
       <c r="I2054" s="53"/>
@@ -30879,7 +31288,7 @@
       <c r="C2055" s="62"/>
       <c r="D2055" s="3"/>
       <c r="E2055" s="53"/>
-      <c r="F2055" s="53"/>
+      <c r="F2055" s="81"/>
       <c r="G2055" s="53"/>
       <c r="H2055" s="53"/>
       <c r="I2055" s="53"/>
@@ -30902,7 +31311,7 @@
       <c r="C2056" s="62"/>
       <c r="D2056" s="3"/>
       <c r="E2056" s="53"/>
-      <c r="F2056" s="53"/>
+      <c r="F2056" s="81"/>
       <c r="G2056" s="53"/>
       <c r="H2056" s="53"/>
       <c r="I2056" s="53"/>
@@ -30925,7 +31334,7 @@
       <c r="C2057" s="62"/>
       <c r="D2057" s="3"/>
       <c r="E2057" s="53"/>
-      <c r="F2057" s="53"/>
+      <c r="F2057" s="81"/>
       <c r="G2057" s="53"/>
       <c r="H2057" s="53"/>
       <c r="I2057" s="53"/>
@@ -30948,7 +31357,7 @@
       <c r="C2058" s="62"/>
       <c r="D2058" s="3"/>
       <c r="E2058" s="53"/>
-      <c r="F2058" s="53"/>
+      <c r="F2058" s="81"/>
       <c r="G2058" s="53"/>
       <c r="H2058" s="53"/>
       <c r="I2058" s="53"/>
@@ -30971,7 +31380,7 @@
       <c r="C2059" s="62"/>
       <c r="D2059" s="3"/>
       <c r="E2059" s="53"/>
-      <c r="F2059" s="53"/>
+      <c r="F2059" s="81"/>
       <c r="G2059" s="53"/>
       <c r="H2059" s="53"/>
       <c r="I2059" s="53"/>
@@ -30994,7 +31403,7 @@
       <c r="C2060" s="62"/>
       <c r="D2060" s="3"/>
       <c r="E2060" s="53"/>
-      <c r="F2060" s="53"/>
+      <c r="F2060" s="81"/>
       <c r="G2060" s="53"/>
       <c r="H2060" s="53"/>
       <c r="I2060" s="53"/>
@@ -31017,7 +31426,7 @@
       <c r="C2061" s="62"/>
       <c r="D2061" s="3"/>
       <c r="E2061" s="53"/>
-      <c r="F2061" s="53"/>
+      <c r="F2061" s="81"/>
       <c r="G2061" s="53"/>
       <c r="H2061" s="53"/>
       <c r="I2061" s="53"/>
@@ -31040,7 +31449,7 @@
       <c r="C2062" s="62"/>
       <c r="D2062" s="3"/>
       <c r="E2062" s="53"/>
-      <c r="F2062" s="53"/>
+      <c r="F2062" s="81"/>
       <c r="G2062" s="53"/>
       <c r="H2062" s="53"/>
       <c r="I2062" s="53"/>
@@ -31063,7 +31472,7 @@
       <c r="C2063" s="62"/>
       <c r="D2063" s="3"/>
       <c r="E2063" s="53"/>
-      <c r="F2063" s="53"/>
+      <c r="F2063" s="81"/>
       <c r="G2063" s="53"/>
       <c r="H2063" s="53"/>
       <c r="I2063" s="53"/>
@@ -31086,7 +31495,7 @@
       <c r="C2064" s="62"/>
       <c r="D2064" s="3"/>
       <c r="E2064" s="53"/>
-      <c r="F2064" s="53"/>
+      <c r="F2064" s="81"/>
       <c r="G2064" s="53"/>
       <c r="H2064" s="53"/>
       <c r="I2064" s="53"/>
@@ -31109,7 +31518,7 @@
       <c r="C2065" s="62"/>
       <c r="D2065" s="3"/>
       <c r="E2065" s="53"/>
-      <c r="F2065" s="53"/>
+      <c r="F2065" s="81"/>
       <c r="G2065" s="53"/>
       <c r="H2065" s="53"/>
       <c r="I2065" s="53"/>
@@ -31132,7 +31541,7 @@
       <c r="C2066" s="62"/>
       <c r="D2066" s="3"/>
       <c r="E2066" s="53"/>
-      <c r="F2066" s="53"/>
+      <c r="F2066" s="81"/>
       <c r="G2066" s="53"/>
       <c r="H2066" s="53"/>
       <c r="I2066" s="53"/>
@@ -31155,7 +31564,7 @@
       <c r="C2067" s="62"/>
       <c r="D2067" s="3"/>
       <c r="E2067" s="53"/>
-      <c r="F2067" s="53"/>
+      <c r="F2067" s="81"/>
       <c r="G2067" s="53"/>
       <c r="H2067" s="53"/>
       <c r="I2067" s="53"/>
@@ -31178,7 +31587,7 @@
       <c r="C2068" s="62"/>
       <c r="D2068" s="3"/>
       <c r="E2068" s="53"/>
-      <c r="F2068" s="53"/>
+      <c r="F2068" s="81"/>
       <c r="G2068" s="53"/>
       <c r="H2068" s="53"/>
       <c r="I2068" s="53"/>
@@ -31201,7 +31610,7 @@
       <c r="C2069" s="62"/>
       <c r="D2069" s="3"/>
       <c r="E2069" s="53"/>
-      <c r="F2069" s="53"/>
+      <c r="F2069" s="81"/>
       <c r="G2069" s="53"/>
       <c r="H2069" s="53"/>
       <c r="I2069" s="53"/>
@@ -31224,7 +31633,7 @@
       <c r="C2070" s="62"/>
       <c r="D2070" s="3"/>
       <c r="E2070" s="53"/>
-      <c r="F2070" s="53"/>
+      <c r="F2070" s="81"/>
       <c r="G2070" s="53"/>
       <c r="H2070" s="53"/>
       <c r="I2070" s="53"/>
@@ -31247,7 +31656,7 @@
       <c r="C2071" s="62"/>
       <c r="D2071" s="3"/>
       <c r="E2071" s="53"/>
-      <c r="F2071" s="53"/>
+      <c r="F2071" s="81"/>
       <c r="G2071" s="53"/>
       <c r="H2071" s="53"/>
       <c r="I2071" s="53"/>
@@ -31270,7 +31679,7 @@
       <c r="C2072" s="62"/>
       <c r="D2072" s="3"/>
       <c r="E2072" s="53"/>
-      <c r="F2072" s="53"/>
+      <c r="F2072" s="81"/>
       <c r="G2072" s="53"/>
       <c r="H2072" s="53"/>
       <c r="I2072" s="53"/>
@@ -31293,7 +31702,7 @@
       <c r="C2073" s="62"/>
       <c r="D2073" s="3"/>
       <c r="E2073" s="53"/>
-      <c r="F2073" s="53"/>
+      <c r="F2073" s="81"/>
       <c r="G2073" s="53"/>
       <c r="H2073" s="53"/>
       <c r="I2073" s="53"/>
@@ -31316,7 +31725,7 @@
       <c r="C2074" s="62"/>
       <c r="D2074" s="3"/>
       <c r="E2074" s="53"/>
-      <c r="F2074" s="53"/>
+      <c r="F2074" s="81"/>
       <c r="G2074" s="53"/>
       <c r="H2074" s="53"/>
       <c r="I2074" s="53"/>
@@ -31339,7 +31748,7 @@
       <c r="C2075" s="62"/>
       <c r="D2075" s="3"/>
       <c r="E2075" s="53"/>
-      <c r="F2075" s="53"/>
+      <c r="F2075" s="81"/>
       <c r="G2075" s="53"/>
       <c r="H2075" s="53"/>
       <c r="I2075" s="53"/>
@@ -31362,7 +31771,7 @@
       <c r="C2076" s="62"/>
       <c r="D2076" s="3"/>
       <c r="E2076" s="53"/>
-      <c r="F2076" s="53"/>
+      <c r="F2076" s="81"/>
       <c r="G2076" s="53"/>
       <c r="H2076" s="53"/>
       <c r="I2076" s="53"/>
@@ -31385,7 +31794,7 @@
       <c r="C2077" s="62"/>
       <c r="D2077" s="3"/>
       <c r="E2077" s="53"/>
-      <c r="F2077" s="53"/>
+      <c r="F2077" s="81"/>
       <c r="G2077" s="53"/>
       <c r="H2077" s="53"/>
       <c r="I2077" s="53"/>
@@ -31408,7 +31817,7 @@
       <c r="C2078" s="62"/>
       <c r="D2078" s="3"/>
       <c r="E2078" s="53"/>
-      <c r="F2078" s="53"/>
+      <c r="F2078" s="81"/>
       <c r="G2078" s="53"/>
       <c r="H2078" s="53"/>
       <c r="I2078" s="53"/>
@@ -31431,7 +31840,7 @@
       <c r="C2079" s="62"/>
       <c r="D2079" s="3"/>
       <c r="E2079" s="53"/>
-      <c r="F2079" s="53"/>
+      <c r="F2079" s="81"/>
       <c r="G2079" s="53"/>
       <c r="H2079" s="53"/>
       <c r="I2079" s="53"/>
@@ -31456,7 +31865,7 @@
         <v>4402</v>
       </c>
       <c r="E2080" s="53"/>
-      <c r="F2080" s="53"/>
+      <c r="F2080" s="81"/>
       <c r="G2080" s="53"/>
       <c r="H2080" s="53"/>
       <c r="I2080" s="53"/>
@@ -31477,7 +31886,7 @@
       <c r="C2081" s="62"/>
       <c r="D2081" s="3"/>
       <c r="E2081" s="53"/>
-      <c r="F2081" s="53"/>
+      <c r="F2081" s="81"/>
       <c r="G2081" s="53"/>
       <c r="H2081" s="53"/>
       <c r="I2081" s="53"/>
@@ -31500,7 +31909,7 @@
       <c r="C2082" s="62"/>
       <c r="D2082" s="3"/>
       <c r="E2082" s="53"/>
-      <c r="F2082" s="53"/>
+      <c r="F2082" s="81"/>
       <c r="G2082" s="53"/>
       <c r="H2082" s="53"/>
       <c r="I2082" s="53"/>
@@ -31523,7 +31932,7 @@
       <c r="C2083" s="62"/>
       <c r="D2083" s="3"/>
       <c r="E2083" s="53"/>
-      <c r="F2083" s="53"/>
+      <c r="F2083" s="81"/>
       <c r="G2083" s="53"/>
       <c r="H2083" s="53"/>
       <c r="I2083" s="53"/>
@@ -31546,7 +31955,7 @@
       <c r="C2084" s="62"/>
       <c r="D2084" s="3"/>
       <c r="E2084" s="53"/>
-      <c r="F2084" s="53"/>
+      <c r="F2084" s="81"/>
       <c r="G2084" s="53"/>
       <c r="H2084" s="53"/>
       <c r="I2084" s="53"/>
@@ -31569,7 +31978,7 @@
       <c r="C2085" s="62"/>
       <c r="D2085" s="3"/>
       <c r="E2085" s="53"/>
-      <c r="F2085" s="53"/>
+      <c r="F2085" s="81"/>
       <c r="G2085" s="53"/>
       <c r="H2085" s="53"/>
       <c r="I2085" s="53"/>
@@ -31592,7 +32001,7 @@
       <c r="C2086" s="62"/>
       <c r="D2086" s="3"/>
       <c r="E2086" s="53"/>
-      <c r="F2086" s="53"/>
+      <c r="F2086" s="81"/>
       <c r="G2086" s="53"/>
       <c r="H2086" s="53"/>
       <c r="I2086" s="53"/>
@@ -31617,7 +32026,7 @@
         <v>4403</v>
       </c>
       <c r="E2087" s="53"/>
-      <c r="F2087" s="53"/>
+      <c r="F2087" s="81"/>
       <c r="G2087" s="53"/>
       <c r="H2087" s="53"/>
       <c r="I2087" s="53"/>
@@ -31638,7 +32047,7 @@
       <c r="C2088" s="62"/>
       <c r="D2088" s="3"/>
       <c r="E2088" s="53"/>
-      <c r="F2088" s="53"/>
+      <c r="F2088" s="81"/>
       <c r="G2088" s="53"/>
       <c r="H2088" s="53"/>
       <c r="I2088" s="53"/>
@@ -31661,7 +32070,7 @@
       <c r="C2089" s="62"/>
       <c r="D2089" s="3"/>
       <c r="E2089" s="53"/>
-      <c r="F2089" s="53"/>
+      <c r="F2089" s="81"/>
       <c r="G2089" s="53"/>
       <c r="H2089" s="53"/>
       <c r="I2089" s="53"/>
@@ -31684,7 +32093,7 @@
       <c r="C2090" s="62"/>
       <c r="D2090" s="3"/>
       <c r="E2090" s="53"/>
-      <c r="F2090" s="53"/>
+      <c r="F2090" s="81"/>
       <c r="G2090" s="53"/>
       <c r="H2090" s="53"/>
       <c r="I2090" s="53"/>
@@ -31707,7 +32116,7 @@
       <c r="C2091" s="62"/>
       <c r="D2091" s="3"/>
       <c r="E2091" s="53"/>
-      <c r="F2091" s="53"/>
+      <c r="F2091" s="81"/>
       <c r="G2091" s="53"/>
       <c r="H2091" s="53"/>
       <c r="I2091" s="53"/>
@@ -31730,7 +32139,7 @@
       <c r="C2092" s="62"/>
       <c r="D2092" s="3"/>
       <c r="E2092" s="53"/>
-      <c r="F2092" s="53"/>
+      <c r="F2092" s="81"/>
       <c r="G2092" s="53"/>
       <c r="H2092" s="53"/>
       <c r="I2092" s="53"/>
@@ -31753,7 +32162,7 @@
       <c r="C2093" s="62"/>
       <c r="D2093" s="3"/>
       <c r="E2093" s="53"/>
-      <c r="F2093" s="53"/>
+      <c r="F2093" s="81"/>
       <c r="G2093" s="53"/>
       <c r="H2093" s="53"/>
       <c r="I2093" s="53"/>
@@ -31776,7 +32185,7 @@
       <c r="C2094" s="62"/>
       <c r="D2094" s="3"/>
       <c r="E2094" s="53"/>
-      <c r="F2094" s="53"/>
+      <c r="F2094" s="81"/>
       <c r="G2094" s="53"/>
       <c r="H2094" s="53"/>
       <c r="I2094" s="53"/>
@@ -31799,7 +32208,7 @@
       <c r="C2095" s="64"/>
       <c r="D2095" s="30"/>
       <c r="E2095" s="65"/>
-      <c r="F2095" s="65"/>
+      <c r="F2095" s="83"/>
       <c r="G2095" s="65"/>
       <c r="H2095" s="65"/>
       <c r="I2095" s="65"/>
@@ -32615,7 +33024,7 @@
       <c r="D2197" s="58" t="s">
         <v>4385</v>
       </c>
-      <c r="F2197" s="22" t="s">
+      <c r="F2197" s="79" t="s">
         <v>4388</v>
       </c>
       <c r="N2197" s="22" t="s">

</xml_diff>